<commit_message>
Actualizacion 1.0 del tablero. Modelo estrella listo
</commit_message>
<xml_diff>
--- a/ALIANZA LIMA 2024.xlsx
+++ b/ALIANZA LIMA 2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056D335E-E2B2-449C-AAEF-860D3469A7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1601D3-8590-46D3-9970-8EC2D3FBD1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -283,12 +283,6 @@
     <t>Waterman</t>
   </si>
   <si>
-    <t>Piero</t>
-  </si>
-  <si>
-    <t>Vivanco</t>
-  </si>
-  <si>
     <t>PAN</t>
   </si>
   <si>
@@ -409,9 +403,6 @@
     <t>Cecilio Waterman</t>
   </si>
   <si>
-    <t>Piero Vivanco</t>
-  </si>
-  <si>
     <t>Sebastián Rodríguez</t>
   </si>
   <si>
@@ -491,6 +482,15 @@
   </si>
   <si>
     <t>Cuando hay gol a favor la motivación sube al máximo. Cuando hay gol del rival la decepción sube al máximo.</t>
+  </si>
+  <si>
+    <t>Cristian Neira</t>
+  </si>
+  <si>
+    <t>Cristian</t>
+  </si>
+  <si>
+    <t>Neira</t>
   </si>
 </sst>
 </file>
@@ -593,7 +593,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="32">
     <dxf>
       <font>
         <color auto="1"/>
@@ -756,46 +756,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <color auto="1"/>
       </font>
       <fill>
@@ -835,44 +795,44 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <color theme="1"/>
+        <b/>
+        <i val="0"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -944,10 +904,10 @@
   </sortState>
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{DF50937B-70CE-4AEE-A127-C34E442E7C61}" name="Nombre Completo" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="28"/>
     <tableColumn id="6" xr3:uid="{1779677D-9229-4A65-A24A-6775E26635BD}" name="Edad 2024"/>
     <tableColumn id="7" xr3:uid="{C7098E7A-A8F5-43C9-A363-2554E8FBB7B3}" name="Pais"/>
     <tableColumn id="8" xr3:uid="{7D8FBA46-C76E-4DB4-B88D-B9B8EDAA5462}" name="Nombres"/>
@@ -958,18 +918,18 @@
     </tableColumn>
     <tableColumn id="12" xr3:uid="{3D8BAAFF-953C-4951-9189-62EB68ED7AD5}" name="Goles"/>
     <tableColumn id="13" xr3:uid="{C1DAD42C-FAD1-46CD-9986-BF72BCE1C663}" name="Asistencias"/>
-    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="27" totalsRowDxfId="20">
+    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="26" totalsRowDxfId="27">
       <calculatedColumnFormula>IFERROR(AVERAGE(T2),"N/A")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{9D730F2E-328A-4494-A682-1BB9B1DAB250}" name="xG. Por partido"/>
     <tableColumn id="16" xr3:uid="{5B84C753-E393-4F3D-B0A0-98D970CA3FEC}" name="xA. Por partido"/>
     <tableColumn id="17" xr3:uid="{1B52557C-9F62-428C-91E9-9F0E11B4F422}" name="Rojas"/>
     <tableColumn id="18" xr3:uid="{0E14E950-7DF2-4515-B85D-A4F9C752C28B}" name="Amarillas"/>
-    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="26" totalsRowDxfId="21"/>
+    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="24" totalsRowDxfId="25"/>
     <tableColumn id="20" xr3:uid="{B764DC06-CAE4-4962-B815-8920EA707CC3}" name="J1 - Rendimiento"/>
-    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="25" totalsRowDxfId="22"/>
+    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="22" totalsRowDxfId="23"/>
     <tableColumn id="22" xr3:uid="{D908F4EA-DBF5-48D1-A49C-6C9FF3E6D4EB}" name="J2 - Rendimiento"/>
-    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="20" totalsRowDxfId="21"/>
     <tableColumn id="24" xr3:uid="{B0AFBAF2-0C32-422F-B101-93952BDD9341}" name="J3 - Rendimiento"/>
     <tableColumn id="25" xr3:uid="{11744F4F-D50A-4354-937A-E6F9873ADF8B}" name="J4 - Minutos"/>
     <tableColumn id="26" xr3:uid="{241981B8-CCE4-4A57-90A2-836FEAC58BA5}" name="J4 - Rendimiento" totalsRowFunction="count"/>
@@ -1281,9 +1241,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B836082-5DF0-4CBD-82AC-74ABD84EC464}">
   <dimension ref="A1:AD27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1309,7 +1269,7 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>70</v>
@@ -1348,13 +1308,13 @@
         <v>46</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="O1" t="s">
+        <v>91</v>
+      </c>
+      <c r="P1" t="s">
         <v>93</v>
-      </c>
-      <c r="P1" t="s">
-        <v>95</v>
       </c>
       <c r="Q1" t="s">
         <v>15</v>
@@ -1363,45 +1323,45 @@
         <v>16</v>
       </c>
       <c r="S1" t="s">
+        <v>121</v>
+      </c>
+      <c r="T1" t="s">
+        <v>123</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
+        <v>125</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" t="s">
         <v>127</v>
       </c>
-      <c r="V1" t="s">
-        <v>128</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="Z1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC1" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="AB1" t="s">
-        <v>140</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>142</v>
-      </c>
       <c r="AD1" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B2" s="5">
         <v>9</v>
@@ -1415,7 +1375,7 @@
         <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H2" t="s">
         <v>38</v>
@@ -1427,7 +1387,7 @@
         <v>40</v>
       </c>
       <c r="K2">
-        <f>SUM(S2,U2,W2)</f>
+        <f t="shared" ref="K2:K27" si="0">SUM(S2,U2,W2)</f>
         <v>270</v>
       </c>
       <c r="L2">
@@ -1437,7 +1397,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="1">
-        <f>IFERROR(AVERAGE(T2),"N/A")</f>
+        <f t="shared" ref="N2:N27" si="1">IFERROR(AVERAGE(T2),"N/A")</f>
         <v>1</v>
       </c>
       <c r="Q2">
@@ -1461,7 +1421,7 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
@@ -1477,7 +1437,7 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H3" t="s">
         <v>41</v>
@@ -1489,7 +1449,7 @@
         <v>26</v>
       </c>
       <c r="K3">
-        <f>SUM(S3,U3,W3)</f>
+        <f t="shared" si="0"/>
         <v>270</v>
       </c>
       <c r="L3">
@@ -1499,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="1">
-        <f>IFERROR(AVERAGE(T3),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q3">
@@ -1523,7 +1483,7 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B4" s="5">
         <v>32</v>
@@ -1537,7 +1497,7 @@
         <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H4" t="s">
         <v>22</v>
@@ -1549,7 +1509,7 @@
         <v>19</v>
       </c>
       <c r="K4">
-        <f>SUM(S4,U4,W4)</f>
+        <f t="shared" si="0"/>
         <v>268</v>
       </c>
       <c r="L4">
@@ -1559,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="1">
-        <f>IFERROR(AVERAGE(T4),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="Q4">
@@ -1586,7 +1546,7 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B5" s="5">
         <v>26</v>
@@ -1604,7 +1564,7 @@
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H5" t="s">
         <v>47</v>
@@ -1616,7 +1576,7 @@
         <v>40</v>
       </c>
       <c r="K5">
-        <f>SUM(S5,U5,W5)</f>
+        <f t="shared" si="0"/>
         <v>255</v>
       </c>
       <c r="L5">
@@ -1626,7 +1586,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="1">
-        <f>IFERROR(AVERAGE(T5),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q5">
@@ -1650,7 +1610,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B6" s="5">
         <v>30</v>
@@ -1666,7 +1626,7 @@
         <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H6" t="s">
         <v>78</v>
@@ -1678,7 +1638,7 @@
         <v>40</v>
       </c>
       <c r="K6">
-        <f>SUM(S6,U6,W6)</f>
+        <f t="shared" si="0"/>
         <v>248</v>
       </c>
       <c r="L6">
@@ -1688,7 +1648,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="1">
-        <f>IFERROR(AVERAGE(T6),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q6">
@@ -1715,7 +1675,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B7" s="5">
         <v>29</v>
@@ -1727,16 +1687,16 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F7">
         <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I7" t="s">
         <v>60</v>
@@ -1745,7 +1705,7 @@
         <v>26</v>
       </c>
       <c r="K7">
-        <f>SUM(S7,U7,W7)</f>
+        <f t="shared" si="0"/>
         <v>246</v>
       </c>
       <c r="L7">
@@ -1755,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="1">
-        <f>IFERROR(AVERAGE(T7),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="Q7">
@@ -1779,7 +1739,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B8" s="5">
         <v>10</v>
@@ -1795,19 +1755,19 @@
         <v>31</v>
       </c>
       <c r="G8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J8" t="s">
         <v>31</v>
       </c>
       <c r="K8">
-        <f>SUM(S8,U8,W8)</f>
+        <f t="shared" si="0"/>
         <v>234</v>
       </c>
       <c r="L8">
@@ -1817,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="1">
-        <f>IFERROR(AVERAGE(T8),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q8">
@@ -1841,7 +1801,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B9" s="5">
         <v>27</v>
@@ -1859,7 +1819,7 @@
         <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H9" t="s">
         <v>56</v>
@@ -1871,7 +1831,7 @@
         <v>31</v>
       </c>
       <c r="K9">
-        <f>SUM(S9,U9,W9)</f>
+        <f t="shared" si="0"/>
         <v>221</v>
       </c>
       <c r="L9">
@@ -1881,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="1">
-        <f>IFERROR(AVERAGE(T9),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q9">
@@ -1905,7 +1865,7 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B10" s="5">
         <v>20</v>
@@ -1923,7 +1883,7 @@
         <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -1935,7 +1895,7 @@
         <v>31</v>
       </c>
       <c r="K10">
-        <f>SUM(S10,U10,W10)</f>
+        <f t="shared" si="0"/>
         <v>199</v>
       </c>
       <c r="L10">
@@ -1945,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="1">
-        <f>IFERROR(AVERAGE(T10),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="Q10">
@@ -1969,7 +1929,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B11" s="5">
         <v>13</v>
@@ -1987,7 +1947,7 @@
         <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H11" t="s">
         <v>27</v>
@@ -1999,7 +1959,7 @@
         <v>26</v>
       </c>
       <c r="K11">
-        <f>SUM(S11,U11,W11)</f>
+        <f t="shared" si="0"/>
         <v>176</v>
       </c>
       <c r="L11">
@@ -2009,7 +1969,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="1">
-        <f>IFERROR(AVERAGE(T11),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>-0.5</v>
       </c>
       <c r="Q11">
@@ -2033,7 +1993,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B12" s="5">
         <v>5</v>
@@ -2051,7 +2011,7 @@
         <v>31</v>
       </c>
       <c r="G12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H12" t="s">
         <v>58</v>
@@ -2063,7 +2023,7 @@
         <v>31</v>
       </c>
       <c r="K12">
-        <f>SUM(S12,U12,W12)</f>
+        <f t="shared" si="0"/>
         <v>148</v>
       </c>
       <c r="L12">
@@ -2073,7 +2033,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="1">
-        <f>IFERROR(AVERAGE(T12),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="Q12">
@@ -2089,7 +2049,7 @@
         <v>-2</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="W12" s="1">
         <v>90</v>
@@ -2097,7 +2057,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B13" s="5">
         <v>18</v>
@@ -2115,7 +2075,7 @@
         <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H13" t="s">
         <v>62</v>
@@ -2127,7 +2087,7 @@
         <v>31</v>
       </c>
       <c r="K13">
-        <f>SUM(S13,U13,W13)</f>
+        <f t="shared" si="0"/>
         <v>91</v>
       </c>
       <c r="L13">
@@ -2137,7 +2097,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="1">
-        <f>IFERROR(AVERAGE(T13),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q13">
@@ -2161,7 +2121,7 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B14" s="5">
         <v>15</v>
@@ -2179,7 +2139,7 @@
         <v>28</v>
       </c>
       <c r="G14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H14" t="s">
         <v>32</v>
@@ -2191,7 +2151,7 @@
         <v>31</v>
       </c>
       <c r="K14">
-        <f>SUM(S14,U14,W14)</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
       <c r="L14">
@@ -2201,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="N14" s="1">
-        <f>IFERROR(AVERAGE(T14),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q14">
@@ -2220,12 +2180,12 @@
         <v>63</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B15" s="5">
         <v>6</v>
@@ -2234,14 +2194,14 @@
         <v>5</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15">
         <v>28</v>
       </c>
       <c r="G15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H15" t="s">
         <v>54</v>
@@ -2253,7 +2213,7 @@
         <v>26</v>
       </c>
       <c r="K15">
-        <f>SUM(S15,U15,W15)</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="L15">
@@ -2263,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="1">
-        <f>IFERROR(AVERAGE(T15),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q15">
@@ -2287,7 +2247,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B16" s="5">
         <v>8</v>
@@ -2305,7 +2265,7 @@
         <v>34</v>
       </c>
       <c r="G16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H16" t="s">
         <v>34</v>
@@ -2317,7 +2277,7 @@
         <v>31</v>
       </c>
       <c r="K16">
-        <f>SUM(S16,U16,W16)</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="L16">
@@ -2327,7 +2287,7 @@
         <v>0</v>
       </c>
       <c r="N16" s="1">
-        <f>IFERROR(AVERAGE(T16),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q16">
@@ -2351,7 +2311,7 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B17" s="5">
         <v>7</v>
@@ -2369,7 +2329,7 @@
         <v>24</v>
       </c>
       <c r="G17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H17" t="s">
         <v>22</v>
@@ -2381,7 +2341,7 @@
         <v>31</v>
       </c>
       <c r="K17">
-        <f>SUM(S17,U17,W17)</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="L17">
@@ -2391,7 +2351,7 @@
         <v>0</v>
       </c>
       <c r="N17" s="1">
-        <f>IFERROR(AVERAGE(T17),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q17">
@@ -2407,7 +2367,7 @@
         <v>0</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="W17" s="1">
         <v>26</v>
@@ -2415,7 +2375,7 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B18" s="5">
         <v>14</v>
@@ -2431,7 +2391,7 @@
         <v>23</v>
       </c>
       <c r="G18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H18" t="s">
         <v>50</v>
@@ -2443,7 +2403,7 @@
         <v>31</v>
       </c>
       <c r="K18">
-        <f>SUM(S18,U18,W18)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="L18">
@@ -2453,7 +2413,7 @@
         <v>0</v>
       </c>
       <c r="N18" s="1" t="str">
-        <f>IFERROR(AVERAGE(T18),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>N/A</v>
       </c>
       <c r="Q18">
@@ -2463,7 +2423,7 @@
         <v>1</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="U18" s="1">
         <v>18</v>
@@ -2472,12 +2432,12 @@
         <v>-0.5</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B19" s="5">
         <v>25</v>
@@ -2493,19 +2453,19 @@
         <v>21</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I19" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J19" t="s">
         <v>26</v>
       </c>
       <c r="K19">
-        <f>SUM(S19,U19,W19)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="L19">
@@ -2515,7 +2475,7 @@
         <v>0</v>
       </c>
       <c r="N19" s="1" t="str">
-        <f>IFERROR(AVERAGE(T19),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>N/A</v>
       </c>
       <c r="Q19">
@@ -2525,10 +2485,10 @@
         <v>0</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="W19" s="1">
         <v>14</v>
@@ -2536,7 +2496,7 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
@@ -2550,7 +2510,7 @@
         <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H20" t="s">
         <v>17</v>
@@ -2562,7 +2522,7 @@
         <v>19</v>
       </c>
       <c r="K20">
-        <f>SUM(S20,U20,W20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L20">
@@ -2572,7 +2532,7 @@
         <v>0</v>
       </c>
       <c r="N20" s="1" t="str">
-        <f>IFERROR(AVERAGE(T20),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>N/A</v>
       </c>
       <c r="Q20">
@@ -2582,24 +2542,24 @@
         <v>0</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="AA20" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="AC20" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B21" s="5">
         <v>12</v>
@@ -2613,7 +2573,7 @@
         <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H21" t="s">
         <v>20</v>
@@ -2625,7 +2585,7 @@
         <v>19</v>
       </c>
       <c r="K21">
-        <f>SUM(S21,U21,W21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L21">
@@ -2635,7 +2595,7 @@
         <v>0</v>
       </c>
       <c r="N21" s="1">
-        <f>IFERROR(AVERAGE(T21),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q21">
@@ -2657,12 +2617,12 @@
         <v>0</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B22" s="5">
         <v>4</v>
@@ -2678,7 +2638,7 @@
         <v>19</v>
       </c>
       <c r="G22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H22" t="s">
         <v>24</v>
@@ -2690,7 +2650,7 @@
         <v>26</v>
       </c>
       <c r="K22">
-        <f>SUM(S22,U22,W22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L22">
@@ -2700,7 +2660,7 @@
         <v>0</v>
       </c>
       <c r="N22" s="1">
-        <f>IFERROR(AVERAGE(T22),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q22">
@@ -2724,7 +2684,7 @@
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B23" s="5">
         <v>31</v>
@@ -2740,7 +2700,7 @@
         <v>29</v>
       </c>
       <c r="G23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H23" t="s">
         <v>29</v>
@@ -2752,7 +2712,7 @@
         <v>26</v>
       </c>
       <c r="K23">
-        <f>SUM(S23,U23,W23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L23">
@@ -2762,7 +2722,7 @@
         <v>0</v>
       </c>
       <c r="N23" s="1">
-        <f>IFERROR(AVERAGE(T23),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q23">
@@ -2786,7 +2746,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B24" s="5">
         <v>19</v>
@@ -2802,7 +2762,7 @@
         <v>27</v>
       </c>
       <c r="G24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H24" t="s">
         <v>36</v>
@@ -2814,7 +2774,7 @@
         <v>40</v>
       </c>
       <c r="K24">
-        <f>SUM(S24,U24,W24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L24">
@@ -2824,7 +2784,7 @@
         <v>0</v>
       </c>
       <c r="N24" s="1" t="str">
-        <f>IFERROR(AVERAGE(T24),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>N/A</v>
       </c>
       <c r="Q24">
@@ -2834,15 +2794,15 @@
         <v>0</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B25" s="5">
         <v>24</v>
@@ -2858,7 +2818,7 @@
         <v>17</v>
       </c>
       <c r="G25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H25" t="s">
         <v>44</v>
@@ -2870,7 +2830,7 @@
         <v>40</v>
       </c>
       <c r="K25">
-        <f>SUM(S25,U25,W25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L25">
@@ -2880,7 +2840,7 @@
         <v>0</v>
       </c>
       <c r="N25" s="1" t="str">
-        <f>IFERROR(AVERAGE(T25),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>N/A</v>
       </c>
       <c r="Q25">
@@ -2890,43 +2850,36 @@
         <v>0</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="B26" s="5">
         <v>16</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26">
-        <v>24</v>
-      </c>
       <c r="G26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H26" t="s">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="I26" t="s">
-        <v>81</v>
+        <v>149</v>
       </c>
       <c r="J26" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="K26">
-        <f>SUM(S26,U26,W26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L26">
@@ -2936,7 +2889,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="1">
-        <f>IFERROR(AVERAGE(T26),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q26">
@@ -2945,25 +2898,25 @@
       <c r="R26">
         <v>0</v>
       </c>
-      <c r="S26" s="1">
-        <v>0</v>
+      <c r="S26" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="T26">
         <v>0</v>
       </c>
-      <c r="U26" s="1">
-        <v>0</v>
+      <c r="U26" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="V26">
         <v>0</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B27" s="5">
         <v>21</v>
@@ -2979,19 +2932,19 @@
         <v>20</v>
       </c>
       <c r="G27" t="s">
+        <v>82</v>
+      </c>
+      <c r="H27" t="s">
         <v>84</v>
       </c>
-      <c r="H27" t="s">
-        <v>86</v>
-      </c>
       <c r="I27" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J27" t="s">
         <v>26</v>
       </c>
       <c r="K27">
-        <f>SUM(S27,U27,W27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L27">
@@ -3001,7 +2954,7 @@
         <v>0</v>
       </c>
       <c r="N27" s="1" t="str">
-        <f>IFERROR(AVERAGE(T27),"N/A")</f>
+        <f t="shared" si="1"/>
         <v>N/A</v>
       </c>
       <c r="Q27">
@@ -3011,7 +2964,7 @@
         <v>0</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="U27" s="1">
         <v>0</v>
@@ -3021,67 +2974,67 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="S2:S27 U2:U27 W2:W27">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+  <conditionalFormatting sqref="W2:W27 S2:S27 U2:U27">
+    <cfRule type="cellIs" dxfId="3" priority="13" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="15" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="16" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y20">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA20">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC20">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3098,7 +3051,7 @@
   <dimension ref="B2:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3113,22 +3066,22 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -3140,45 +3093,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C662F49D-D799-4554-A671-6CB45781BA74}">
   <dimension ref="B2:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grafico de dispersion de edad alianza lima
</commit_message>
<xml_diff>
--- a/ALIANZA LIMA 2024.xlsx
+++ b/ALIANZA LIMA 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1601D3-8590-46D3-9970-8EC2D3FBD1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA7E3B5-F9C0-4CD2-8184-39F2F8AAD55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$Z$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$Z$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="153">
   <si>
     <t>POR</t>
   </si>
@@ -491,6 +491,15 @@
   </si>
   <si>
     <t>Neira</t>
+  </si>
+  <si>
+    <t>Víctor Guzmán</t>
+  </si>
+  <si>
+    <t>Víctor</t>
+  </si>
+  <si>
+    <t>Guzmán</t>
   </si>
 </sst>
 </file>
@@ -568,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -589,11 +598,492 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="80">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -897,17 +1387,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D01F760-0D73-4C44-A79F-5468B2DB0477}" name="AlianzaLima" displayName="AlianzaLima" ref="A1:AD27">
-  <autoFilter ref="A1:AD27" xr:uid="{7B836082-5DF0-4CBD-82AC-74ABD84EC464}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D01F760-0D73-4C44-A79F-5468B2DB0477}" name="AlianzaLima" displayName="AlianzaLima" ref="A1:AD28">
+  <autoFilter ref="A1:AD28" xr:uid="{7B836082-5DF0-4CBD-82AC-74ABD84EC464}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z27">
     <sortCondition descending="1" ref="K1:K27"/>
   </sortState>
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{DF50937B-70CE-4AEE-A127-C34E442E7C61}" name="Nombre Completo" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="76"/>
     <tableColumn id="6" xr3:uid="{1779677D-9229-4A65-A24A-6775E26635BD}" name="Edad 2024"/>
     <tableColumn id="7" xr3:uid="{C7098E7A-A8F5-43C9-A363-2554E8FBB7B3}" name="Pais"/>
     <tableColumn id="8" xr3:uid="{7D8FBA46-C76E-4DB4-B88D-B9B8EDAA5462}" name="Nombres"/>
@@ -918,18 +1408,18 @@
     </tableColumn>
     <tableColumn id="12" xr3:uid="{3D8BAAFF-953C-4951-9189-62EB68ED7AD5}" name="Goles"/>
     <tableColumn id="13" xr3:uid="{C1DAD42C-FAD1-46CD-9986-BF72BCE1C663}" name="Asistencias"/>
-    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="26" totalsRowDxfId="27">
+    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="75" totalsRowDxfId="74">
       <calculatedColumnFormula>IFERROR(AVERAGE(T2),"N/A")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{9D730F2E-328A-4494-A682-1BB9B1DAB250}" name="xG. Por partido"/>
     <tableColumn id="16" xr3:uid="{5B84C753-E393-4F3D-B0A0-98D970CA3FEC}" name="xA. Por partido"/>
     <tableColumn id="17" xr3:uid="{1B52557C-9F62-428C-91E9-9F0E11B4F422}" name="Rojas"/>
     <tableColumn id="18" xr3:uid="{0E14E950-7DF2-4515-B85D-A4F9C752C28B}" name="Amarillas"/>
-    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="24" totalsRowDxfId="25"/>
+    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="73" totalsRowDxfId="72"/>
     <tableColumn id="20" xr3:uid="{B764DC06-CAE4-4962-B815-8920EA707CC3}" name="J1 - Rendimiento"/>
-    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="22" totalsRowDxfId="23"/>
+    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="71" totalsRowDxfId="70"/>
     <tableColumn id="22" xr3:uid="{D908F4EA-DBF5-48D1-A49C-6C9FF3E6D4EB}" name="J2 - Rendimiento"/>
-    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="20" totalsRowDxfId="21"/>
+    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="69" totalsRowDxfId="68"/>
     <tableColumn id="24" xr3:uid="{B0AFBAF2-0C32-422F-B101-93952BDD9341}" name="J3 - Rendimiento"/>
     <tableColumn id="25" xr3:uid="{11744F4F-D50A-4354-937A-E6F9873ADF8B}" name="J4 - Minutos"/>
     <tableColumn id="26" xr3:uid="{241981B8-CCE4-4A57-90A2-836FEAC58BA5}" name="J4 - Rendimiento" totalsRowFunction="count"/>
@@ -1239,11 +1729,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B836082-5DF0-4CBD-82AC-74ABD84EC464}">
-  <dimension ref="A1:AD27"/>
+  <dimension ref="A1:AD28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A26" sqref="A26"/>
+      <selection pane="topRight" activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2465,7 +2955,7 @@
         <v>26</v>
       </c>
       <c r="K19">
-        <f t="shared" si="0"/>
+        <f>SUM(S19,U19,W19)</f>
         <v>14</v>
       </c>
       <c r="L19">
@@ -2973,68 +3463,101 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" s="5">
+        <v>22</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28">
+        <v>18</v>
+      </c>
+      <c r="G28" t="s">
+        <v>82</v>
+      </c>
+      <c r="H28" t="s">
+        <v>151</v>
+      </c>
+      <c r="I28" t="s">
+        <v>152</v>
+      </c>
+      <c r="J28" t="s">
+        <v>40</v>
+      </c>
+      <c r="K28">
+        <f>SUM(S28,U28,W28)</f>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1" t="str">
+        <f>IFERROR(AVERAGE(T28),"N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y28" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="W2:W27 S2:S27 U2:U27">
-    <cfRule type="cellIs" dxfId="3" priority="13" operator="equal">
+  <conditionalFormatting sqref="W2:W28 S2:S28 U2:U28">
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="14" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y20">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+  <conditionalFormatting sqref="Y2:Y28 AA2:AA28 AC2:AC28">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA20">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
-      <formula>90</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="between">
-      <formula>6</formula>
-      <formula>89</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="between">
-      <formula>0</formula>
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC20">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
-      <formula>90</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="between">
-      <formula>6</formula>
-      <formula>89</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="between">
-      <formula>0</formula>
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3144,7 +3667,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
automatizada la carga de los archivos por jornada al archivo principal. Minutos, Goles, Asistencias
</commit_message>
<xml_diff>
--- a/ALIANZA LIMA 2024.xlsx
+++ b/ALIANZA LIMA 2024.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA7E3B5-F9C0-4CD2-8184-39F2F8AAD55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0EB8E3-5DFD-419F-A220-7C4EB00D9F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
     <sheet name="Jornada 1" sheetId="4" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$Z$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Jugadores!$A$1:$Z$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="154">
   <si>
     <t>POR</t>
   </si>
@@ -232,9 +232,6 @@
     <t>Jhamir</t>
   </si>
   <si>
-    <t>D'arrigo</t>
-  </si>
-  <si>
     <t>DFI</t>
   </si>
   <si>
@@ -358,18 +355,12 @@
     <t>Ángel De la Cruz</t>
   </si>
   <si>
-    <t>Nicolás Amasifuén</t>
-  </si>
-  <si>
     <t>Ricardo Lagos</t>
   </si>
   <si>
     <t>Yordi Vílchez</t>
   </si>
   <si>
-    <t>Jesús Castillo Peña</t>
-  </si>
-  <si>
     <t>Gabriel Costa</t>
   </si>
   <si>
@@ -388,18 +379,12 @@
     <t>Kevin Serna</t>
   </si>
   <si>
-    <t>Renzo Garcés</t>
-  </si>
-  <si>
     <t>Catriel Cabellos</t>
   </si>
   <si>
     <t>Jiovany Ramos</t>
   </si>
   <si>
-    <t>Juan Pablo Freytes</t>
-  </si>
-  <si>
     <t>Cecilio Waterman</t>
   </si>
   <si>
@@ -409,9 +394,6 @@
     <t>J1 - Minutos</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>J1 - Rendimiento</t>
   </si>
   <si>
@@ -439,9 +421,6 @@
     <t>J4 - Rendimiento</t>
   </si>
   <si>
-    <t>Jhamir D'Arrigo</t>
-  </si>
-  <si>
     <t>Marco Huaman</t>
   </si>
   <si>
@@ -500,6 +479,30 @@
   </si>
   <si>
     <t>Guzmán</t>
+  </si>
+  <si>
+    <t>J7 -  Minutos</t>
+  </si>
+  <si>
+    <t>J7 - Rendimiento</t>
+  </si>
+  <si>
+    <t>Darrigo</t>
+  </si>
+  <si>
+    <t>Juan Freytes</t>
+  </si>
+  <si>
+    <t>Jesús Castillo</t>
+  </si>
+  <si>
+    <t>Renzo Garces</t>
+  </si>
+  <si>
+    <t>Nicolas Amasifuen</t>
+  </si>
+  <si>
+    <t>Jhamir D´Arrigo</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -541,6 +544,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor theme="4"/>
       </patternFill>
     </fill>
@@ -577,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -595,234 +610,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="18">
     <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <color theme="1"/>
+        <b/>
+        <i val="0"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -883,446 +722,6 @@
           <bgColor theme="9"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1387,39 +786,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D01F760-0D73-4C44-A79F-5468B2DB0477}" name="AlianzaLima" displayName="AlianzaLima" ref="A1:AD28">
-  <autoFilter ref="A1:AD28" xr:uid="{7B836082-5DF0-4CBD-82AC-74ABD84EC464}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D01F760-0D73-4C44-A79F-5468B2DB0477}" name="AlianzaLima" displayName="AlianzaLima" ref="A1:AF28">
+  <autoFilter ref="A1:AF28" xr:uid="{7B836082-5DF0-4CBD-82AC-74ABD84EC464}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z27">
     <sortCondition descending="1" ref="K1:K27"/>
   </sortState>
-  <tableColumns count="30">
+  <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{DF50937B-70CE-4AEE-A127-C34E442E7C61}" name="Nombre Completo" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{1779677D-9229-4A65-A24A-6775E26635BD}" name="Edad 2024"/>
     <tableColumn id="7" xr3:uid="{C7098E7A-A8F5-43C9-A363-2554E8FBB7B3}" name="Pais"/>
     <tableColumn id="8" xr3:uid="{7D8FBA46-C76E-4DB4-B88D-B9B8EDAA5462}" name="Nombres"/>
     <tableColumn id="9" xr3:uid="{BEEDC3B4-9AB7-4927-B473-ED8A7E1F4766}" name="Apellidos"/>
     <tableColumn id="10" xr3:uid="{9AA904B3-4DD8-4262-BFAD-8331FA5E7FBD}" name="Posición"/>
-    <tableColumn id="11" xr3:uid="{A731302C-3B92-4B73-9269-9251FFF431F7}" name="Minutos">
-      <calculatedColumnFormula>SUM(S2,U2,W2)</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="11" xr3:uid="{A731302C-3B92-4B73-9269-9251FFF431F7}" name="Minutos"/>
     <tableColumn id="12" xr3:uid="{3D8BAAFF-953C-4951-9189-62EB68ED7AD5}" name="Goles"/>
     <tableColumn id="13" xr3:uid="{C1DAD42C-FAD1-46CD-9986-BF72BCE1C663}" name="Asistencias"/>
-    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="75" totalsRowDxfId="74">
-      <calculatedColumnFormula>IFERROR(AVERAGE(T2),"N/A")</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="7" totalsRowDxfId="6"/>
     <tableColumn id="15" xr3:uid="{9D730F2E-328A-4494-A682-1BB9B1DAB250}" name="xG. Por partido"/>
     <tableColumn id="16" xr3:uid="{5B84C753-E393-4F3D-B0A0-98D970CA3FEC}" name="xA. Por partido"/>
     <tableColumn id="17" xr3:uid="{1B52557C-9F62-428C-91E9-9F0E11B4F422}" name="Rojas"/>
     <tableColumn id="18" xr3:uid="{0E14E950-7DF2-4515-B85D-A4F9C752C28B}" name="Amarillas"/>
-    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="5" totalsRowDxfId="4"/>
     <tableColumn id="20" xr3:uid="{B764DC06-CAE4-4962-B815-8920EA707CC3}" name="J1 - Rendimiento"/>
-    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="3" totalsRowDxfId="2"/>
     <tableColumn id="22" xr3:uid="{D908F4EA-DBF5-48D1-A49C-6C9FF3E6D4EB}" name="J2 - Rendimiento"/>
-    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="1" totalsRowDxfId="0"/>
     <tableColumn id="24" xr3:uid="{B0AFBAF2-0C32-422F-B101-93952BDD9341}" name="J3 - Rendimiento"/>
     <tableColumn id="25" xr3:uid="{11744F4F-D50A-4354-937A-E6F9873ADF8B}" name="J4 - Minutos"/>
     <tableColumn id="26" xr3:uid="{241981B8-CCE4-4A57-90A2-836FEAC58BA5}" name="J4 - Rendimiento" totalsRowFunction="count"/>
@@ -1427,6 +822,8 @@
     <tableColumn id="28" xr3:uid="{3C611F36-9630-4D04-B092-C9A01E082439}" name="J5 - Rendimiento"/>
     <tableColumn id="29" xr3:uid="{C60003FA-AFE3-475D-9049-216E7B944915}" name="J6 -  Minutos"/>
     <tableColumn id="30" xr3:uid="{685FC9C5-8519-434E-810E-4C0CF8B07E7B}" name="J6 - Rendimiento"/>
+    <tableColumn id="31" xr3:uid="{78007039-1AC2-40FF-99C0-9F2670CD2130}" name="J7 -  Minutos"/>
+    <tableColumn id="32" xr3:uid="{EFF3CC86-8062-41DB-828E-0E6884E98DC4}" name="J7 - Rendimiento"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -1729,11 +1126,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B836082-5DF0-4CBD-82AC-74ABD84EC464}">
-  <dimension ref="A1:AD28"/>
+  <dimension ref="A1:AF28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z2" sqref="Z2"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1755,14 +1152,16 @@
     <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1774,7 +1173,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
@@ -1788,23 +1187,23 @@
       <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="8" t="s">
         <v>46</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P1" t="s">
         <v>92</v>
-      </c>
-      <c r="O1" t="s">
-        <v>91</v>
-      </c>
-      <c r="P1" t="s">
-        <v>93</v>
       </c>
       <c r="Q1" t="s">
         <v>15</v>
@@ -1812,46 +1211,52 @@
       <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="T1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="V1" t="s">
+        <v>119</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="X1" t="s">
         <v>121</v>
       </c>
-      <c r="T1" t="s">
-        <v>123</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
         <v>125</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="X1" t="s">
-        <v>127</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB1" t="s">
         <v>130</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD1" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE1" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B2" s="5">
         <v>9</v>
@@ -1865,7 +1270,7 @@
         <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H2" t="s">
         <v>38</v>
@@ -1877,17 +1282,15 @@
         <v>40</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K27" si="0">SUM(S2,U2,W2)</f>
-        <v>270</v>
+        <v>424</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N2" s="1">
-        <f t="shared" ref="N2:N27" si="1">IFERROR(AVERAGE(T2),"N/A")</f>
         <v>1</v>
       </c>
       <c r="Q2">
@@ -1908,16 +1311,22 @@
       <c r="W2" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Y2">
+        <v>90</v>
+      </c>
+      <c r="AA2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>5</v>
@@ -1927,7 +1336,7 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H3" t="s">
         <v>41</v>
@@ -1939,8 +1348,7 @@
         <v>26</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
-        <v>270</v>
+        <v>450</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1949,7 +1357,6 @@
         <v>0</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q3">
@@ -1970,10 +1377,16 @@
       <c r="W3" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Y3">
+        <v>90</v>
+      </c>
+      <c r="AA3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="5">
         <v>32</v>
@@ -1987,7 +1400,7 @@
         <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H4" t="s">
         <v>22</v>
@@ -1999,8 +1412,7 @@
         <v>19</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
-        <v>268</v>
+        <v>359</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -2009,8 +1421,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Q4">
         <v>1</v>
@@ -2022,21 +1433,24 @@
         <v>90</v>
       </c>
       <c r="T4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="U4" s="1">
         <v>90</v>
       </c>
       <c r="W4" s="1">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="X4">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="AA4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B5" s="5">
         <v>26</v>
@@ -2048,13 +1462,13 @@
         <v>53</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5">
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H5" t="s">
         <v>47</v>
@@ -2066,17 +1480,15 @@
         <v>40</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
-        <v>255</v>
+        <v>409</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q5">
@@ -2097,10 +1509,16 @@
       <c r="W5" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Y5">
+        <v>90</v>
+      </c>
+      <c r="AA5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B6" s="5">
         <v>30</v>
@@ -2116,29 +1534,27 @@
         <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" t="s">
         <v>78</v>
-      </c>
-      <c r="I6" t="s">
-        <v>79</v>
       </c>
       <c r="J6" t="s">
         <v>40</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
-        <v>248</v>
+        <v>421</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q6">
@@ -2162,10 +1578,16 @@
       <c r="W6" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Y6">
+        <v>83</v>
+      </c>
+      <c r="AA6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B7" s="5">
         <v>29</v>
@@ -2177,16 +1599,16 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F7">
         <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I7" t="s">
         <v>60</v>
@@ -2195,8 +1617,7 @@
         <v>26</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
-        <v>246</v>
+        <v>336</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -2205,8 +1626,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Q7">
         <v>1</v>
@@ -2218,7 +1638,7 @@
         <v>90</v>
       </c>
       <c r="T7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="U7" s="1">
         <v>90</v>
@@ -2226,16 +1646,19 @@
       <c r="W7" s="1">
         <v>66</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B8" s="5">
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>53</v>
@@ -2245,20 +1668,19 @@
         <v>31</v>
       </c>
       <c r="G8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" t="s">
         <v>84</v>
-      </c>
-      <c r="I8" t="s">
-        <v>85</v>
       </c>
       <c r="J8" t="s">
         <v>31</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
-        <v>234</v>
+        <v>392</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -2267,7 +1689,6 @@
         <v>0</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q8">
@@ -2288,19 +1709,25 @@
       <c r="W8" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Y8">
+        <v>74</v>
+      </c>
+      <c r="AA8">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B9" s="5">
         <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>8</v>
@@ -2309,7 +1736,7 @@
         <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H9" t="s">
         <v>56</v>
@@ -2321,17 +1748,15 @@
         <v>31</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
-        <v>221</v>
+        <v>323</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q9">
@@ -2352,10 +1777,16 @@
       <c r="W9" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Y9">
+        <v>84</v>
+      </c>
+      <c r="AA9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="5">
         <v>20</v>
@@ -2364,16 +1795,16 @@
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="F10">
         <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -2385,8 +1816,7 @@
         <v>31</v>
       </c>
       <c r="K10">
-        <f t="shared" si="0"/>
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -2395,8 +1825,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="1">
-        <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -2408,7 +1837,7 @@
         <v>90</v>
       </c>
       <c r="T10">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="U10" s="1">
         <v>64</v>
@@ -2416,10 +1845,16 @@
       <c r="W10" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Y10">
+        <v>16</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B11" s="5">
         <v>13</v>
@@ -2428,16 +1863,16 @@
         <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F11">
         <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H11" t="s">
         <v>27</v>
@@ -2449,8 +1884,7 @@
         <v>26</v>
       </c>
       <c r="K11">
-        <f t="shared" si="0"/>
-        <v>176</v>
+        <v>338</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -2459,8 +1893,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -2472,7 +1905,7 @@
         <v>90</v>
       </c>
       <c r="T11">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="U11" s="1">
         <v>72</v>
@@ -2480,28 +1913,34 @@
       <c r="W11" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Y11">
+        <v>90</v>
+      </c>
+      <c r="AA11">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="5">
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="F12">
         <v>31</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H12" t="s">
         <v>58</v>
@@ -2513,18 +1952,16 @@
         <v>31</v>
       </c>
       <c r="K12">
-        <f t="shared" si="0"/>
-        <v>148</v>
+        <v>328</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="Q12">
         <v>1</v>
@@ -2536,49 +1973,52 @@
         <v>58</v>
       </c>
       <c r="T12">
-        <v>-2</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>122</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="U12" s="2"/>
       <c r="W12" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Y12">
+        <v>90</v>
+      </c>
+      <c r="AA12">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="B13" s="5">
         <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="F13">
         <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H13" t="s">
         <v>62</v>
       </c>
       <c r="I13" t="s">
-        <v>63</v>
+        <v>148</v>
       </c>
       <c r="J13" t="s">
         <v>31</v>
       </c>
       <c r="K13">
-        <f t="shared" si="0"/>
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -2587,7 +2027,6 @@
         <v>1</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q13">
@@ -2608,28 +2047,34 @@
       <c r="W13" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="B14" s="5">
         <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="F14">
         <v>28</v>
       </c>
       <c r="G14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H14" t="s">
         <v>32</v>
@@ -2641,8 +2086,7 @@
         <v>31</v>
       </c>
       <c r="K14">
-        <f t="shared" si="0"/>
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -2651,7 +2095,6 @@
         <v>1</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q14">
@@ -2669,13 +2112,19 @@
       <c r="U14" s="1">
         <v>63</v>
       </c>
-      <c r="W14" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="W14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>28</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="B15" s="5">
         <v>6</v>
@@ -2684,14 +2133,14 @@
         <v>5</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15">
         <v>28</v>
       </c>
       <c r="G15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H15" t="s">
         <v>54</v>
@@ -2703,8 +2152,7 @@
         <v>26</v>
       </c>
       <c r="K15">
-        <f t="shared" si="0"/>
-        <v>72</v>
+        <v>252</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -2713,7 +2161,6 @@
         <v>0</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q15">
@@ -2734,28 +2181,34 @@
       <c r="W15" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="Y15">
+        <v>90</v>
+      </c>
+      <c r="AA15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B16" s="5">
         <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="F16">
         <v>34</v>
       </c>
       <c r="G16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H16" t="s">
         <v>34</v>
@@ -2767,17 +2220,15 @@
         <v>31</v>
       </c>
       <c r="K16">
-        <f t="shared" si="0"/>
-        <v>56</v>
+        <v>202</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q16">
@@ -2798,10 +2249,16 @@
       <c r="W16" s="1">
         <v>45</v>
       </c>
+      <c r="Y16">
+        <v>62</v>
+      </c>
+      <c r="AA16">
+        <v>84</v>
+      </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B17" s="5">
         <v>7</v>
@@ -2813,13 +2270,13 @@
         <v>52</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F17">
         <v>24</v>
       </c>
       <c r="G17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H17" t="s">
         <v>22</v>
@@ -2831,17 +2288,15 @@
         <v>31</v>
       </c>
       <c r="K17">
-        <f t="shared" si="0"/>
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="1">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q17">
@@ -2856,32 +2311,36 @@
       <c r="T17">
         <v>0</v>
       </c>
-      <c r="U17" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="U17" s="2"/>
       <c r="W17" s="1">
         <v>26</v>
       </c>
+      <c r="Y17">
+        <v>11</v>
+      </c>
+      <c r="AA17">
+        <v>26</v>
+      </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" s="5">
         <v>14</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18">
         <v>23</v>
       </c>
       <c r="G18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H18" t="s">
         <v>50</v>
@@ -2893,8 +2352,7 @@
         <v>31</v>
       </c>
       <c r="K18">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -2902,32 +2360,33 @@
       <c r="M18">
         <v>0</v>
       </c>
-      <c r="N18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>N/A</v>
-      </c>
+      <c r="N18" s="1"/>
       <c r="Q18">
         <v>0</v>
       </c>
       <c r="R18">
         <v>1</v>
       </c>
-      <c r="S18" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="S18" s="2"/>
       <c r="U18" s="1">
         <v>18</v>
       </c>
       <c r="V18">
-        <v>-0.5</v>
-      </c>
-      <c r="W18" s="1" t="s">
-        <v>122</v>
+        <v>0.5</v>
+      </c>
+      <c r="W18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>10</v>
+      </c>
+      <c r="AA18">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B19" s="5">
         <v>25</v>
@@ -2943,19 +2402,18 @@
         <v>21</v>
       </c>
       <c r="G19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H19" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="I19" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="J19" t="s">
         <v>26</v>
       </c>
       <c r="K19">
-        <f>SUM(S19,U19,W19)</f>
         <v>14</v>
       </c>
       <c r="L19">
@@ -2964,29 +2422,28 @@
       <c r="M19">
         <v>0</v>
       </c>
-      <c r="N19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>N/A</v>
-      </c>
+      <c r="N19" s="1"/>
       <c r="Q19">
         <v>0</v>
       </c>
       <c r="R19">
         <v>0</v>
       </c>
-      <c r="S19" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="U19" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="S19" s="2"/>
+      <c r="U19" s="2"/>
       <c r="W19" s="1">
         <v>14</v>
       </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
@@ -3000,7 +2457,7 @@
         <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H20" t="s">
         <v>17</v>
@@ -3012,7 +2469,6 @@
         <v>19</v>
       </c>
       <c r="K20">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L20">
@@ -3021,35 +2477,21 @@
       <c r="M20">
         <v>0</v>
       </c>
-      <c r="N20" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>N/A</v>
-      </c>
+      <c r="N20" s="1"/>
       <c r="Q20">
         <v>0</v>
       </c>
       <c r="R20">
         <v>0</v>
       </c>
-      <c r="S20" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="U20" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y20" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AA20" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AC20" s="6" t="s">
-        <v>122</v>
-      </c>
+      <c r="S20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AC20" s="6"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" s="5">
         <v>12</v>
@@ -3063,7 +2505,7 @@
         <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H21" t="s">
         <v>20</v>
@@ -3075,8 +2517,7 @@
         <v>19</v>
       </c>
       <c r="K21">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -3085,7 +2526,6 @@
         <v>0</v>
       </c>
       <c r="N21" s="1">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q21">
@@ -3106,19 +2546,25 @@
       <c r="V21">
         <v>0</v>
       </c>
-      <c r="W21" s="1" t="s">
-        <v>122</v>
+      <c r="W21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>90</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>152</v>
       </c>
       <c r="B22" s="5">
         <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>7</v>
@@ -3128,7 +2574,7 @@
         <v>19</v>
       </c>
       <c r="G22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H22" t="s">
         <v>24</v>
@@ -3140,7 +2586,6 @@
         <v>26</v>
       </c>
       <c r="K22">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L22">
@@ -3150,7 +2595,6 @@
         <v>0</v>
       </c>
       <c r="N22" s="1">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q22">
@@ -3169,12 +2613,15 @@
         <v>0</v>
       </c>
       <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B23" s="5">
         <v>31</v>
@@ -3190,7 +2637,7 @@
         <v>29</v>
       </c>
       <c r="G23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H23" t="s">
         <v>29</v>
@@ -3202,7 +2649,6 @@
         <v>26</v>
       </c>
       <c r="K23">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L23">
@@ -3212,7 +2658,6 @@
         <v>0</v>
       </c>
       <c r="N23" s="1">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q23">
@@ -3236,7 +2681,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B24" s="5">
         <v>19</v>
@@ -3245,14 +2690,14 @@
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24">
         <v>27</v>
       </c>
       <c r="G24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H24" t="s">
         <v>36</v>
@@ -3264,7 +2709,6 @@
         <v>40</v>
       </c>
       <c r="K24">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L24">
@@ -3273,26 +2717,19 @@
       <c r="M24">
         <v>0</v>
       </c>
-      <c r="N24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>N/A</v>
-      </c>
+      <c r="N24" s="1"/>
       <c r="Q24">
         <v>0</v>
       </c>
       <c r="R24">
         <v>0</v>
       </c>
-      <c r="S24" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="U24" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="S24" s="2"/>
+      <c r="U24" s="2"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B25" s="5">
         <v>24</v>
@@ -3308,7 +2745,7 @@
         <v>17</v>
       </c>
       <c r="G25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H25" t="s">
         <v>44</v>
@@ -3320,7 +2757,6 @@
         <v>40</v>
       </c>
       <c r="K25">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L25">
@@ -3329,26 +2765,19 @@
       <c r="M25">
         <v>0</v>
       </c>
-      <c r="N25" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>N/A</v>
-      </c>
+      <c r="N25" s="1"/>
       <c r="Q25">
         <v>0</v>
       </c>
       <c r="R25">
         <v>0</v>
       </c>
-      <c r="S25" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="U25" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="S25" s="2"/>
+      <c r="U25" s="2"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B26" s="5">
         <v>16</v>
@@ -3357,19 +2786,18 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="G26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H26" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="I26" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="J26" t="s">
         <v>31</v>
       </c>
       <c r="K26">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L26">
@@ -3379,7 +2807,6 @@
         <v>0</v>
       </c>
       <c r="N26" s="1">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q26">
@@ -3388,31 +2815,24 @@
       <c r="R26">
         <v>0</v>
       </c>
-      <c r="S26" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="S26" s="2"/>
       <c r="T26">
         <v>0</v>
       </c>
-      <c r="U26" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="U26" s="2"/>
       <c r="V26">
         <v>0</v>
-      </c>
-      <c r="W26" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B27" s="5">
         <v>21</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>7</v>
@@ -3422,19 +2842,18 @@
         <v>20</v>
       </c>
       <c r="G27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I27" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="J27" t="s">
         <v>26</v>
       </c>
       <c r="K27">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L27">
@@ -3443,19 +2862,14 @@
       <c r="M27">
         <v>0</v>
       </c>
-      <c r="N27" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>N/A</v>
-      </c>
+      <c r="N27" s="1"/>
       <c r="Q27">
         <v>0</v>
       </c>
       <c r="R27">
         <v>0</v>
       </c>
-      <c r="S27" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="S27" s="2"/>
       <c r="U27" s="1">
         <v>0</v>
       </c>
@@ -3465,7 +2879,7 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B28" s="5">
         <v>22</v>
@@ -3474,27 +2888,26 @@
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28">
         <v>18</v>
       </c>
       <c r="G28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H28" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="I28" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="J28" t="s">
         <v>40</v>
       </c>
       <c r="K28">
-        <f>SUM(S28,U28,W28)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -3502,63 +2915,44 @@
       <c r="M28">
         <v>0</v>
       </c>
-      <c r="N28" s="1" t="str">
-        <f>IFERROR(AVERAGE(T28),"N/A")</f>
-        <v>N/A</v>
-      </c>
+      <c r="N28" s="1"/>
       <c r="Q28">
         <v>0</v>
       </c>
       <c r="R28">
         <v>0</v>
       </c>
-      <c r="S28" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="U28" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y28" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>122</v>
+      <c r="S28" s="1"/>
+      <c r="Y28" s="7"/>
+      <c r="AA28">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="W2:W28 S2:S28 U2:U28">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+  <conditionalFormatting sqref="W2:W28 S2:S28 U2:U28 Y2:Y28">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y28 AA2:AA28 AC2:AC28">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="AA2:AA28 AC2:AC28">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="between">
       <formula>0</formula>
       <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
-      <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3589,22 +2983,22 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
         <v>96</v>
       </c>
-      <c r="C2" t="s">
-        <v>97</v>
-      </c>
       <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
         <v>89</v>
       </c>
-      <c r="E2" t="s">
-        <v>90</v>
-      </c>
       <c r="F2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" t="s">
         <v>94</v>
-      </c>
-      <c r="G2" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -3624,37 +3018,37 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios en el entorno
</commit_message>
<xml_diff>
--- a/ALIANZA LIMA 2024.xlsx
+++ b/ALIANZA LIMA 2024.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0EB8E3-5DFD-419F-A220-7C4EB00D9F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCB3B91-DEBD-4C49-904B-F986B1181223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
-    <sheet name="Jornada 1" sheetId="4" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId4"/>
+    <sheet name="Jornadas" sheetId="5" r:id="rId2"/>
+    <sheet name="Jornada 1" sheetId="4" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Jugadores!$A$1:$Z$28</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="170">
   <si>
     <t>POR</t>
   </si>
@@ -100,9 +101,6 @@
     <t>Campos</t>
   </si>
   <si>
-    <t>Arquero</t>
-  </si>
-  <si>
     <t>Ángel</t>
   </si>
   <si>
@@ -334,9 +332,6 @@
     <t>Cantidad de remates con destino a arco</t>
   </si>
   <si>
-    <t>Nombre Completo</t>
-  </si>
-  <si>
     <t>Aldair Fuentes</t>
   </si>
   <si>
@@ -487,9 +482,6 @@
     <t>J7 - Rendimiento</t>
   </si>
   <si>
-    <t>Darrigo</t>
-  </si>
-  <si>
     <t>Juan Freytes</t>
   </si>
   <si>
@@ -503,13 +495,70 @@
   </si>
   <si>
     <t>Jhamir D´Arrigo</t>
+  </si>
+  <si>
+    <t>Jugador</t>
+  </si>
+  <si>
+    <t>Portero</t>
+  </si>
+  <si>
+    <t>D'Arrigo</t>
+  </si>
+  <si>
+    <t>Jornada</t>
+  </si>
+  <si>
+    <t>Condicion</t>
+  </si>
+  <si>
+    <t>Jornada 1 - Local vs Universidad Cesar Vallejo</t>
+  </si>
+  <si>
+    <t>Jornada 2 - Visita vs Alianza Atlético de Sullana</t>
+  </si>
+  <si>
+    <t>Jornada 3 - Local vs Universitario de Deportes</t>
+  </si>
+  <si>
+    <t>Jornada 4 - Visita vs Unión Comercio</t>
+  </si>
+  <si>
+    <t>Jornada 5 - Local vs Comerciantes Unidos</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Visita</t>
+  </si>
+  <si>
+    <t>Jornada 6 - Visita vs ADT</t>
+  </si>
+  <si>
+    <t>Importancia</t>
+  </si>
+  <si>
+    <t>Apertura</t>
+  </si>
+  <si>
+    <t>Torneo</t>
+  </si>
+  <si>
+    <t>ID Jornada</t>
+  </si>
+  <si>
+    <t>Posicion resultante</t>
+  </si>
+  <si>
+    <t>Jornada 7 - Local vs Sporting Cristal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,6 +581,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -560,7 +614,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -588,11 +642,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -618,51 +687,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -722,6 +754,46 @@
           <bgColor theme="9"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -792,11 +864,11 @@
     <sortCondition descending="1" ref="K1:K27"/>
   </sortState>
   <tableColumns count="32">
-    <tableColumn id="1" xr3:uid="{DF50937B-70CE-4AEE-A127-C34E442E7C61}" name="Nombre Completo" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{DF50937B-70CE-4AEE-A127-C34E442E7C61}" name="Jugador" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="14"/>
     <tableColumn id="6" xr3:uid="{1779677D-9229-4A65-A24A-6775E26635BD}" name="Edad 2024"/>
     <tableColumn id="7" xr3:uid="{C7098E7A-A8F5-43C9-A363-2554E8FBB7B3}" name="Pais"/>
     <tableColumn id="8" xr3:uid="{7D8FBA46-C76E-4DB4-B88D-B9B8EDAA5462}" name="Nombres"/>
@@ -805,16 +877,16 @@
     <tableColumn id="11" xr3:uid="{A731302C-3B92-4B73-9269-9251FFF431F7}" name="Minutos"/>
     <tableColumn id="12" xr3:uid="{3D8BAAFF-953C-4951-9189-62EB68ED7AD5}" name="Goles"/>
     <tableColumn id="13" xr3:uid="{C1DAD42C-FAD1-46CD-9986-BF72BCE1C663}" name="Asistencias"/>
-    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="12" totalsRowDxfId="13"/>
     <tableColumn id="15" xr3:uid="{9D730F2E-328A-4494-A682-1BB9B1DAB250}" name="xG. Por partido"/>
     <tableColumn id="16" xr3:uid="{5B84C753-E393-4F3D-B0A0-98D970CA3FEC}" name="xA. Por partido"/>
     <tableColumn id="17" xr3:uid="{1B52557C-9F62-428C-91E9-9F0E11B4F422}" name="Rojas"/>
     <tableColumn id="18" xr3:uid="{0E14E950-7DF2-4515-B85D-A4F9C752C28B}" name="Amarillas"/>
-    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="10" totalsRowDxfId="11"/>
     <tableColumn id="20" xr3:uid="{B764DC06-CAE4-4962-B815-8920EA707CC3}" name="J1 - Rendimiento"/>
-    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="8" totalsRowDxfId="9"/>
     <tableColumn id="22" xr3:uid="{D908F4EA-DBF5-48D1-A49C-6C9FF3E6D4EB}" name="J2 - Rendimiento"/>
-    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="6" totalsRowDxfId="7"/>
     <tableColumn id="24" xr3:uid="{B0AFBAF2-0C32-422F-B101-93952BDD9341}" name="J3 - Rendimiento"/>
     <tableColumn id="25" xr3:uid="{11744F4F-D50A-4354-937A-E6F9873ADF8B}" name="J4 - Minutos"/>
     <tableColumn id="26" xr3:uid="{241981B8-CCE4-4A57-90A2-836FEAC58BA5}" name="J4 - Rendimiento" totalsRowFunction="count"/>
@@ -1130,7 +1202,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="AC18" sqref="AC18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1158,10 +1230,10 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1173,7 +1245,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
@@ -1194,16 +1266,16 @@
         <v>14</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P1" t="s">
         <v>91</v>
-      </c>
-      <c r="O1" t="s">
-        <v>90</v>
-      </c>
-      <c r="P1" t="s">
-        <v>92</v>
       </c>
       <c r="Q1" t="s">
         <v>15</v>
@@ -1212,51 +1284,51 @@
         <v>16</v>
       </c>
       <c r="S1" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="T1" t="s">
+        <v>115</v>
+      </c>
+      <c r="U1" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>117</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>119</v>
       </c>
-      <c r="W1" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="X1" t="s">
-        <v>121</v>
-      </c>
       <c r="Y1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Z1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AA1" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD1" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="AB1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="AE1" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" s="5">
         <v>9</v>
@@ -1270,16 +1342,16 @@
         <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
         <v>38</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>39</v>
-      </c>
-      <c r="J2" t="s">
-        <v>40</v>
       </c>
       <c r="K2">
         <v>424</v>
@@ -1320,13 +1392,13 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>5</v>
@@ -1336,16 +1408,16 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K3">
         <v>450</v>
@@ -1386,7 +1458,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" s="5">
         <v>32</v>
@@ -1400,16 +1472,16 @@
         <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="K4">
         <v>359</v>
@@ -1438,6 +1510,9 @@
       <c r="U4" s="1">
         <v>90</v>
       </c>
+      <c r="V4">
+        <v>-2</v>
+      </c>
       <c r="W4" s="1">
         <v>89</v>
       </c>
@@ -1450,34 +1525,34 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" s="5">
         <v>26</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F5">
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" t="s">
         <v>47</v>
       </c>
-      <c r="I5" t="s">
-        <v>48</v>
-      </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K5">
         <v>409</v>
@@ -1518,13 +1593,13 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B6" s="5">
         <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>9</v>
@@ -1534,16 +1609,16 @@
         <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" t="s">
         <v>77</v>
       </c>
-      <c r="I6" t="s">
-        <v>78</v>
-      </c>
       <c r="J6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K6">
         <v>421</v>
@@ -1587,7 +1662,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B7" s="5">
         <v>29</v>
@@ -1599,22 +1674,22 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F7">
         <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K7">
         <v>336</v>
@@ -1652,32 +1727,32 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B8" s="5">
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8">
         <v>31</v>
       </c>
       <c r="G8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H8" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" t="s">
         <v>83</v>
       </c>
-      <c r="I8" t="s">
-        <v>84</v>
-      </c>
       <c r="J8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K8">
         <v>392</v>
@@ -1718,16 +1793,16 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B9" s="5">
         <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>8</v>
@@ -1736,16 +1811,16 @@
         <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" t="s">
         <v>56</v>
       </c>
-      <c r="I9" t="s">
-        <v>57</v>
-      </c>
       <c r="J9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K9">
         <v>323</v>
@@ -1786,7 +1861,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B10" s="5">
         <v>20</v>
@@ -1795,25 +1870,25 @@
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="F10">
         <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K10">
         <v>215</v>
@@ -1854,7 +1929,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B11" s="5">
         <v>13</v>
@@ -1863,25 +1938,25 @@
         <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11">
         <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" t="s">
         <v>27</v>
       </c>
-      <c r="I11" t="s">
-        <v>28</v>
-      </c>
       <c r="J11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K11">
         <v>338</v>
@@ -1922,34 +1997,34 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B12" s="5">
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="F12">
         <v>31</v>
       </c>
       <c r="G12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" t="s">
         <v>58</v>
       </c>
-      <c r="I12" t="s">
-        <v>59</v>
-      </c>
       <c r="J12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K12">
         <v>328</v>
@@ -1988,34 +2063,34 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B13" s="5">
         <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="F13">
         <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I13" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="J13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K13">
         <v>117</v>
@@ -2056,34 +2131,34 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B14" s="5">
         <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="F14">
         <v>28</v>
       </c>
       <c r="G14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" t="s">
         <v>32</v>
       </c>
-      <c r="I14" t="s">
-        <v>33</v>
-      </c>
       <c r="J14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K14">
         <v>113</v>
@@ -2124,7 +2199,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B15" s="5">
         <v>6</v>
@@ -2133,23 +2208,23 @@
         <v>5</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15">
         <v>28</v>
       </c>
       <c r="G15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H15" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" t="s">
         <v>54</v>
       </c>
-      <c r="I15" t="s">
-        <v>55</v>
-      </c>
       <c r="J15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K15">
         <v>252</v>
@@ -2190,34 +2265,34 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B16" s="5">
         <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="F16">
         <v>34</v>
       </c>
       <c r="G16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" t="s">
         <v>34</v>
       </c>
-      <c r="I16" t="s">
-        <v>35</v>
-      </c>
       <c r="J16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K16">
         <v>202</v>
@@ -2258,7 +2333,7 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B17" s="5">
         <v>7</v>
@@ -2267,25 +2342,25 @@
         <v>8</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F17">
         <v>24</v>
       </c>
       <c r="G17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K17">
         <v>85</v>
@@ -2324,32 +2399,32 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B18" s="5">
         <v>14</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18">
         <v>23</v>
       </c>
       <c r="G18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H18" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" t="s">
         <v>50</v>
       </c>
-      <c r="I18" t="s">
-        <v>51</v>
-      </c>
       <c r="J18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K18">
         <v>38</v>
@@ -2386,7 +2461,7 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B19" s="5">
         <v>25</v>
@@ -2402,16 +2477,16 @@
         <v>21</v>
       </c>
       <c r="G19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K19">
         <v>14</v>
@@ -2443,7 +2518,7 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
@@ -2457,7 +2532,7 @@
         <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H20" t="s">
         <v>17</v>
@@ -2466,7 +2541,7 @@
         <v>18</v>
       </c>
       <c r="J20" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -2491,7 +2566,7 @@
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B21" s="5">
         <v>12</v>
@@ -2505,16 +2580,16 @@
         <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" t="s">
         <v>20</v>
       </c>
-      <c r="I21" t="s">
-        <v>21</v>
-      </c>
       <c r="J21" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="K21">
         <v>90</v>
@@ -2558,13 +2633,13 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B22" s="5">
         <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>7</v>
@@ -2574,16 +2649,16 @@
         <v>19</v>
       </c>
       <c r="G22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H22" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" t="s">
         <v>24</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>25</v>
-      </c>
-      <c r="J22" t="s">
-        <v>26</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -2621,7 +2696,7 @@
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B23" s="5">
         <v>31</v>
@@ -2637,16 +2712,16 @@
         <v>29</v>
       </c>
       <c r="G23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" t="s">
         <v>29</v>
       </c>
-      <c r="I23" t="s">
-        <v>30</v>
-      </c>
       <c r="J23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -2681,7 +2756,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B24" s="5">
         <v>19</v>
@@ -2690,23 +2765,23 @@
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24">
         <v>27</v>
       </c>
       <c r="G24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -2729,7 +2804,7 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B25" s="5">
         <v>24</v>
@@ -2738,23 +2813,23 @@
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25">
         <v>17</v>
       </c>
       <c r="G25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" t="s">
         <v>44</v>
       </c>
-      <c r="I25" t="s">
-        <v>45</v>
-      </c>
       <c r="J25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -2777,25 +2852,29 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B26" s="5">
         <v>16</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="G26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H26" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -2826,13 +2905,13 @@
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B27" s="5">
         <v>21</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>7</v>
@@ -2842,16 +2921,16 @@
         <v>20</v>
       </c>
       <c r="G27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -2879,7 +2958,7 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B28" s="5">
         <v>22</v>
@@ -2888,23 +2967,23 @@
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28">
         <v>18</v>
       </c>
       <c r="G28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I28" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K28">
         <v>10</v>
@@ -2930,27 +3009,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W2:W28 S2:S28 U2:U28 Y2:Y28">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="14" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="15" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA28 AC2:AC28">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
@@ -2964,6 +3043,182 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01D9F4C-E000-464C-8ABC-D44BFB0FC070}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="39.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534A273A-43EF-4B78-8C56-DAE3EB14BBD5}">
   <dimension ref="B2:G2"/>
   <sheetViews>
@@ -2983,22 +3238,22 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
         <v>95</v>
       </c>
-      <c r="C2" t="s">
-        <v>96</v>
-      </c>
       <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
         <v>88</v>
       </c>
-      <c r="E2" t="s">
-        <v>89</v>
-      </c>
       <c r="F2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" t="s">
         <v>93</v>
-      </c>
-      <c r="G2" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -3006,7 +3261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C662F49D-D799-4554-A671-6CB45781BA74}">
   <dimension ref="B2:B13"/>
   <sheetViews>
@@ -3018,37 +3273,37 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -3056,7 +3311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C54044-AF01-4FF7-B5B5-75D3A52CE000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
arreglamos el tablero final, creado en main_app.py
</commit_message>
<xml_diff>
--- a/ALIANZA LIMA 2024.xlsx
+++ b/ALIANZA LIMA 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCB3B91-DEBD-4C49-904B-F986B1181223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE21C42-FA7D-498C-A35A-06E79D28EDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
   </bookViews>
@@ -434,9 +434,6 @@
     <t>J6 - Rendimiento</t>
   </si>
   <si>
-    <t>J6 -  Minutos</t>
-  </si>
-  <si>
     <t>para analizar el futbol se necesitan</t>
   </si>
   <si>
@@ -476,9 +473,6 @@
     <t>Guzmán</t>
   </si>
   <si>
-    <t>J7 -  Minutos</t>
-  </si>
-  <si>
     <t>J7 - Rendimiento</t>
   </si>
   <si>
@@ -552,6 +546,12 @@
   </si>
   <si>
     <t>Jornada 7 - Local vs Sporting Cristal</t>
+  </si>
+  <si>
+    <t>J6 - Minutos</t>
+  </si>
+  <si>
+    <t>J7 - Minutos</t>
   </si>
 </sst>
 </file>
@@ -696,6 +696,46 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color theme="1"/>
       </font>
@@ -754,46 +794,6 @@
           <bgColor theme="9"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -865,10 +865,10 @@
   </sortState>
   <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{DF50937B-70CE-4AEE-A127-C34E442E7C61}" name="Jugador" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{1779677D-9229-4A65-A24A-6775E26635BD}" name="Edad 2024"/>
     <tableColumn id="7" xr3:uid="{C7098E7A-A8F5-43C9-A363-2554E8FBB7B3}" name="Pais"/>
     <tableColumn id="8" xr3:uid="{7D8FBA46-C76E-4DB4-B88D-B9B8EDAA5462}" name="Nombres"/>
@@ -877,24 +877,24 @@
     <tableColumn id="11" xr3:uid="{A731302C-3B92-4B73-9269-9251FFF431F7}" name="Minutos"/>
     <tableColumn id="12" xr3:uid="{3D8BAAFF-953C-4951-9189-62EB68ED7AD5}" name="Goles"/>
     <tableColumn id="13" xr3:uid="{C1DAD42C-FAD1-46CD-9986-BF72BCE1C663}" name="Asistencias"/>
-    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="12" totalsRowDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="7" totalsRowDxfId="6"/>
     <tableColumn id="15" xr3:uid="{9D730F2E-328A-4494-A682-1BB9B1DAB250}" name="xG. Por partido"/>
     <tableColumn id="16" xr3:uid="{5B84C753-E393-4F3D-B0A0-98D970CA3FEC}" name="xA. Por partido"/>
     <tableColumn id="17" xr3:uid="{1B52557C-9F62-428C-91E9-9F0E11B4F422}" name="Rojas"/>
     <tableColumn id="18" xr3:uid="{0E14E950-7DF2-4515-B85D-A4F9C752C28B}" name="Amarillas"/>
-    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="5" totalsRowDxfId="4"/>
     <tableColumn id="20" xr3:uid="{B764DC06-CAE4-4962-B815-8920EA707CC3}" name="J1 - Rendimiento"/>
-    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="3" totalsRowDxfId="2"/>
     <tableColumn id="22" xr3:uid="{D908F4EA-DBF5-48D1-A49C-6C9FF3E6D4EB}" name="J2 - Rendimiento"/>
-    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="1" totalsRowDxfId="0"/>
     <tableColumn id="24" xr3:uid="{B0AFBAF2-0C32-422F-B101-93952BDD9341}" name="J3 - Rendimiento"/>
     <tableColumn id="25" xr3:uid="{11744F4F-D50A-4354-937A-E6F9873ADF8B}" name="J4 - Minutos"/>
     <tableColumn id="26" xr3:uid="{241981B8-CCE4-4A57-90A2-836FEAC58BA5}" name="J4 - Rendimiento" totalsRowFunction="count"/>
     <tableColumn id="27" xr3:uid="{1F8DD667-456E-4B4E-812F-806054078F00}" name="J5 - Minutos"/>
     <tableColumn id="28" xr3:uid="{3C611F36-9630-4D04-B092-C9A01E082439}" name="J5 - Rendimiento"/>
-    <tableColumn id="29" xr3:uid="{C60003FA-AFE3-475D-9049-216E7B944915}" name="J6 -  Minutos"/>
+    <tableColumn id="29" xr3:uid="{C60003FA-AFE3-475D-9049-216E7B944915}" name="J6 - Minutos"/>
     <tableColumn id="30" xr3:uid="{685FC9C5-8519-434E-810E-4C0CF8B07E7B}" name="J6 - Rendimiento"/>
-    <tableColumn id="31" xr3:uid="{78007039-1AC2-40FF-99C0-9F2670CD2130}" name="J7 -  Minutos"/>
+    <tableColumn id="31" xr3:uid="{78007039-1AC2-40FF-99C0-9F2670CD2130}" name="J7 - Minutos"/>
     <tableColumn id="32" xr3:uid="{EFF3CC86-8062-41DB-828E-0E6884E98DC4}" name="J7 - Rendimiento"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
@@ -1202,7 +1202,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AC18" sqref="AC18"/>
+      <selection pane="topRight" activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1230,7 +1230,7 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>68</v>
@@ -1314,16 +1314,16 @@
         <v>128</v>
       </c>
       <c r="AC1" s="10" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="AD1" s="4" t="s">
         <v>129</v>
       </c>
       <c r="AE1" s="10" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
@@ -1354,7 +1354,7 @@
         <v>39</v>
       </c>
       <c r="K2">
-        <v>424</v>
+        <v>469</v>
       </c>
       <c r="L2">
         <v>2</v>
@@ -1389,10 +1389,13 @@
       <c r="AA2">
         <v>64</v>
       </c>
+      <c r="AC2">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
@@ -1420,7 +1423,7 @@
         <v>25</v>
       </c>
       <c r="K3">
-        <v>450</v>
+        <v>540</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1453,6 +1456,9 @@
         <v>90</v>
       </c>
       <c r="AA3">
+        <v>90</v>
+      </c>
+      <c r="AC3">
         <v>90</v>
       </c>
     </row>
@@ -1481,10 +1487,10 @@
         <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K4">
-        <v>359</v>
+        <v>384</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1521,6 +1527,9 @@
       </c>
       <c r="AA4">
         <v>90</v>
+      </c>
+      <c r="AC4">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
@@ -1555,7 +1564,7 @@
         <v>39</v>
       </c>
       <c r="K5">
-        <v>409</v>
+        <v>499</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -1589,6 +1598,9 @@
       </c>
       <c r="AA5">
         <v>64</v>
+      </c>
+      <c r="AC5">
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
@@ -1621,7 +1633,7 @@
         <v>39</v>
       </c>
       <c r="K6">
-        <v>421</v>
+        <v>506</v>
       </c>
       <c r="L6">
         <v>3</v>
@@ -1658,6 +1670,9 @@
       </c>
       <c r="AA6">
         <v>90</v>
+      </c>
+      <c r="AC6">
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
@@ -1692,7 +1707,7 @@
         <v>25</v>
       </c>
       <c r="K7">
-        <v>336</v>
+        <v>426</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1722,6 +1737,9 @@
         <v>66</v>
       </c>
       <c r="AA7">
+        <v>90</v>
+      </c>
+      <c r="AC7">
         <v>90</v>
       </c>
     </row>
@@ -1755,7 +1773,7 @@
         <v>30</v>
       </c>
       <c r="K8">
-        <v>392</v>
+        <v>482</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -1789,6 +1807,9 @@
       </c>
       <c r="AA8">
         <v>84</v>
+      </c>
+      <c r="AC8">
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
@@ -1858,6 +1879,9 @@
       <c r="AA9">
         <v>18</v>
       </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1926,6 +1950,9 @@
       <c r="AA10">
         <v>0</v>
       </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -2027,7 +2054,7 @@
         <v>30</v>
       </c>
       <c r="K12">
-        <v>328</v>
+        <v>418</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -2060,10 +2087,13 @@
       <c r="AA12">
         <v>90</v>
       </c>
+      <c r="AC12">
+        <v>90</v>
+      </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B13" s="5">
         <v>18</v>
@@ -2087,13 +2117,13 @@
         <v>61</v>
       </c>
       <c r="I13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J13" t="s">
         <v>25</v>
       </c>
       <c r="K13">
-        <v>117</v>
+        <v>186</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -2128,10 +2158,13 @@
       <c r="AA13">
         <v>26</v>
       </c>
+      <c r="AC13">
+        <v>69</v>
+      </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B14" s="5">
         <v>15</v>
@@ -2161,7 +2194,7 @@
         <v>30</v>
       </c>
       <c r="K14">
-        <v>113</v>
+        <v>158</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -2196,10 +2229,13 @@
       <c r="AA14">
         <v>0</v>
       </c>
+      <c r="AC14">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B15" s="5">
         <v>6</v>
@@ -2227,7 +2263,7 @@
         <v>25</v>
       </c>
       <c r="K15">
-        <v>252</v>
+        <v>342</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -2260,6 +2296,9 @@
         <v>90</v>
       </c>
       <c r="AA15">
+        <v>90</v>
+      </c>
+      <c r="AC15">
         <v>90</v>
       </c>
     </row>
@@ -2295,7 +2334,7 @@
         <v>30</v>
       </c>
       <c r="K16">
-        <v>202</v>
+        <v>232</v>
       </c>
       <c r="L16">
         <v>1</v>
@@ -2329,6 +2368,9 @@
       </c>
       <c r="AA16">
         <v>84</v>
+      </c>
+      <c r="AC16">
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
@@ -2363,7 +2405,7 @@
         <v>30</v>
       </c>
       <c r="K17">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -2396,6 +2438,9 @@
       <c r="AA17">
         <v>26</v>
       </c>
+      <c r="AC17">
+        <v>21</v>
+      </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -2457,6 +2502,9 @@
       </c>
       <c r="AA18">
         <v>10</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
@@ -2515,6 +2563,9 @@
       <c r="AA19">
         <v>0</v>
       </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -2541,7 +2592,7 @@
         <v>18</v>
       </c>
       <c r="J20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -2589,10 +2640,10 @@
         <v>20</v>
       </c>
       <c r="J21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K21">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -2629,11 +2680,14 @@
       </c>
       <c r="AA21">
         <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B22" s="5">
         <v>4</v>
@@ -2852,7 +2906,7 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B26" s="5">
         <v>16</v>
@@ -2868,10 +2922,10 @@
         <v>80</v>
       </c>
       <c r="H26" t="s">
+        <v>138</v>
+      </c>
+      <c r="I26" t="s">
         <v>139</v>
-      </c>
-      <c r="I26" t="s">
-        <v>140</v>
       </c>
       <c r="J26" t="s">
         <v>30</v>
@@ -2955,10 +3009,13 @@
       <c r="V27">
         <v>0</v>
       </c>
+      <c r="AC27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B28" s="5">
         <v>22</v>
@@ -2977,16 +3034,16 @@
         <v>80</v>
       </c>
       <c r="H28" t="s">
+        <v>141</v>
+      </c>
+      <c r="I28" t="s">
         <v>142</v>
-      </c>
-      <c r="I28" t="s">
-        <v>143</v>
       </c>
       <c r="J28" t="s">
         <v>39</v>
       </c>
       <c r="K28">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -3006,30 +3063,33 @@
       <c r="AA28">
         <v>10</v>
       </c>
+      <c r="AC28">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="W2:W28 S2:S28 U2:U28 Y2:Y28">
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA28 AC2:AC28">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
@@ -3058,39 +3118,39 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>166</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F2">
         <v>4</v>
@@ -3098,19 +3158,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -3118,19 +3178,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D4">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F4">
         <v>7</v>
@@ -3138,19 +3198,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -3158,19 +3218,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -3178,19 +3238,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -3198,19 +3258,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D8">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -3273,37 +3333,37 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimizacion de tablero e importacion de imagenes
</commit_message>
<xml_diff>
--- a/ALIANZA LIMA 2024.xlsx
+++ b/ALIANZA LIMA 2024.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE21C42-FA7D-498C-A35A-06E79D28EDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11ED536F-F737-4982-A4FC-6E26907F83B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
     <sheet name="Jornadas" sheetId="5" r:id="rId2"/>
-    <sheet name="Jornada 1" sheetId="4" r:id="rId3"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId5"/>
+    <sheet name="Categorias" sheetId="6" r:id="rId3"/>
+    <sheet name="Data importante" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Categorias!$A$1:$B$40</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Jugadores!$A$1:$Z$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="217">
   <si>
     <t>POR</t>
   </si>
@@ -552,6 +553,147 @@
   </si>
   <si>
     <t>J7 - Minutos</t>
+  </si>
+  <si>
+    <t>Total de Pases</t>
+  </si>
+  <si>
+    <t>Pases Acertados</t>
+  </si>
+  <si>
+    <t>Total de Balones Largos</t>
+  </si>
+  <si>
+    <t>Balones Largos Acertados</t>
+  </si>
+  <si>
+    <t>Toques</t>
+  </si>
+  <si>
+    <t>Posesion Perdida</t>
+  </si>
+  <si>
+    <t>Pases Clave</t>
+  </si>
+  <si>
+    <t>Total de Centros</t>
+  </si>
+  <si>
+    <t>Centros Acertados</t>
+  </si>
+  <si>
+    <t>Duelos Aereos Perdidos</t>
+  </si>
+  <si>
+    <t>Duelos Aereos Ganados</t>
+  </si>
+  <si>
+    <t>Duelos Perdidos</t>
+  </si>
+  <si>
+    <t>Duelos Ganados</t>
+  </si>
+  <si>
+    <t>Desafios Perdidos</t>
+  </si>
+  <si>
+    <t>Tiros Fuera</t>
+  </si>
+  <si>
+    <t>Despejes Totales</t>
+  </si>
+  <si>
+    <t>Intercepciones Ganadas</t>
+  </si>
+  <si>
+    <t>Entradas Totales</t>
+  </si>
+  <si>
+    <t>Fue Faltado</t>
+  </si>
+  <si>
+    <t>Faltas</t>
+  </si>
+  <si>
+    <t>Total de Fueras de Juego</t>
+  </si>
+  <si>
+    <t>Desposesiones</t>
+  </si>
+  <si>
+    <t>Total de Contiendas</t>
+  </si>
+  <si>
+    <t>Contiendas Ganadas</t>
+  </si>
+  <si>
+    <t>Intentos de Anotacion al Arco</t>
+  </si>
+  <si>
+    <t>Grandes Oportunidades Falladas</t>
+  </si>
+  <si>
+    <t>Intentos de Anotacion Bloqueados</t>
+  </si>
+  <si>
+    <t>Grandes Oportunidades Creadas</t>
+  </si>
+  <si>
+    <t>Balones al Poste</t>
+  </si>
+  <si>
+    <t>Tiros Salvados Dentro del Area</t>
+  </si>
+  <si>
+    <t>Atajadas</t>
+  </si>
+  <si>
+    <t>Penaltis Ganados</t>
+  </si>
+  <si>
+    <t>Penaltis Fallados</t>
+  </si>
+  <si>
+    <t>Errores que Conducen a un Tiro</t>
+  </si>
+  <si>
+    <t>Penaltis Concedidos</t>
+  </si>
+  <si>
+    <t>Bloqueos de Jugadores de Campo</t>
+  </si>
+  <si>
+    <t>Salidas del Portero Totales</t>
+  </si>
+  <si>
+    <t>Salidas de Portero Efectivas</t>
+  </si>
+  <si>
+    <t>Capturas aéreas del balón</t>
+  </si>
+  <si>
+    <t>Porteria</t>
+  </si>
+  <si>
+    <t>Acciones ofensivas</t>
+  </si>
+  <si>
+    <t>Disciplina</t>
+  </si>
+  <si>
+    <t>Concentracion</t>
+  </si>
+  <si>
+    <t>Estadistica</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Acciones defensivas</t>
+  </si>
+  <si>
+    <t>Generacion de juego</t>
   </si>
 </sst>
 </file>
@@ -694,46 +836,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="24">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
+        <color theme="1"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -795,6 +927,76 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -808,55 +1010,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>632460</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>36195</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F9BF55E-4430-F37C-4F18-7BE90A0FE73E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="632460" y="167640"/>
-          <a:ext cx="6705600" cy="4257675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D01F760-0D73-4C44-A79F-5468B2DB0477}" name="AlianzaLima" displayName="AlianzaLima" ref="A1:AF28">
   <autoFilter ref="A1:AF28" xr:uid="{7B836082-5DF0-4CBD-82AC-74ABD84EC464}"/>
@@ -865,10 +1018,10 @@
   </sortState>
   <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{DF50937B-70CE-4AEE-A127-C34E442E7C61}" name="Jugador" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="20"/>
     <tableColumn id="6" xr3:uid="{1779677D-9229-4A65-A24A-6775E26635BD}" name="Edad 2024"/>
     <tableColumn id="7" xr3:uid="{C7098E7A-A8F5-43C9-A363-2554E8FBB7B3}" name="Pais"/>
     <tableColumn id="8" xr3:uid="{7D8FBA46-C76E-4DB4-B88D-B9B8EDAA5462}" name="Nombres"/>
@@ -877,16 +1030,16 @@
     <tableColumn id="11" xr3:uid="{A731302C-3B92-4B73-9269-9251FFF431F7}" name="Minutos"/>
     <tableColumn id="12" xr3:uid="{3D8BAAFF-953C-4951-9189-62EB68ED7AD5}" name="Goles"/>
     <tableColumn id="13" xr3:uid="{C1DAD42C-FAD1-46CD-9986-BF72BCE1C663}" name="Asistencias"/>
-    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="19" totalsRowDxfId="18"/>
     <tableColumn id="15" xr3:uid="{9D730F2E-328A-4494-A682-1BB9B1DAB250}" name="xG. Por partido"/>
     <tableColumn id="16" xr3:uid="{5B84C753-E393-4F3D-B0A0-98D970CA3FEC}" name="xA. Por partido"/>
     <tableColumn id="17" xr3:uid="{1B52557C-9F62-428C-91E9-9F0E11B4F422}" name="Rojas"/>
     <tableColumn id="18" xr3:uid="{0E14E950-7DF2-4515-B85D-A4F9C752C28B}" name="Amarillas"/>
-    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="17" totalsRowDxfId="16"/>
     <tableColumn id="20" xr3:uid="{B764DC06-CAE4-4962-B815-8920EA707CC3}" name="J1 - Rendimiento"/>
-    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="15" totalsRowDxfId="14"/>
     <tableColumn id="22" xr3:uid="{D908F4EA-DBF5-48D1-A49C-6C9FF3E6D4EB}" name="J2 - Rendimiento"/>
-    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="13" totalsRowDxfId="12"/>
     <tableColumn id="24" xr3:uid="{B0AFBAF2-0C32-422F-B101-93952BDD9341}" name="J3 - Rendimiento"/>
     <tableColumn id="25" xr3:uid="{11744F4F-D50A-4354-937A-E6F9873ADF8B}" name="J4 - Minutos"/>
     <tableColumn id="26" xr3:uid="{241981B8-CCE4-4A57-90A2-836FEAC58BA5}" name="J4 - Rendimiento" totalsRowFunction="count"/>
@@ -1202,7 +1355,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R19" sqref="R19"/>
+      <selection pane="topRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1502,7 +1655,7 @@
         <v>1</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -1648,7 +1801,7 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" s="1">
         <v>68</v>
@@ -1788,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S8" s="1">
         <v>68</v>
@@ -1859,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9" s="1">
         <v>90</v>
@@ -2658,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21" s="1">
         <v>0</v>
@@ -2918,6 +3071,9 @@
         <v>71</v>
       </c>
       <c r="E26" s="3"/>
+      <c r="F26">
+        <v>23</v>
+      </c>
       <c r="G26" t="s">
         <v>80</v>
       </c>
@@ -3069,27 +3225,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W2:W28 S2:S28 U2:U28 Y2:Y28">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="14" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="15" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA28 AC2:AC28">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
@@ -3279,6 +3435,352 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DE0E37-A65E-430A-B081-464F0351FE39}">
+  <dimension ref="A1:B40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>196</v>
+      </c>
+      <c r="B6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>180</v>
+      </c>
+      <c r="B11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B18" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>203</v>
+      </c>
+      <c r="B23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>204</v>
+      </c>
+      <c r="B24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>188</v>
+      </c>
+      <c r="B25" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B26" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>172</v>
+      </c>
+      <c r="B29" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>174</v>
+      </c>
+      <c r="B31" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>176</v>
+      </c>
+      <c r="B32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B33" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>178</v>
+      </c>
+      <c r="B34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>197</v>
+      </c>
+      <c r="B35" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>199</v>
+      </c>
+      <c r="B36" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>200</v>
+      </c>
+      <c r="B37" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>206</v>
+      </c>
+      <c r="B38" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>207</v>
+      </c>
+      <c r="B39" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>208</v>
+      </c>
+      <c r="B40" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B40" xr:uid="{F5DE0E37-A65E-430A-B081-464F0351FE39}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B40">
+      <sortCondition ref="B1:B40"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534A273A-43EF-4B78-8C56-DAE3EB14BBD5}">
   <dimension ref="B2:G2"/>
   <sheetViews>
@@ -3321,7 +3823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C662F49D-D799-4554-A671-6CB45781BA74}">
   <dimension ref="B2:B13"/>
   <sheetViews>
@@ -3369,19 +3871,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C54044-AF01-4FF7-B5B5-75D3A52CE000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Obtenemos archivos generales hasta J8
</commit_message>
<xml_diff>
--- a/ALIANZA LIMA 2024.xlsx
+++ b/ALIANZA LIMA 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11ED536F-F737-4982-A4FC-6E26907F83B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8427246B-F457-4338-819F-19C35D318BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="218">
   <si>
     <t>POR</t>
   </si>
@@ -694,6 +694,9 @@
   </si>
   <si>
     <t>Generacion de juego</t>
+  </si>
+  <si>
+    <t>Jornada 8 - Visita vs Cienciano</t>
   </si>
 </sst>
 </file>
@@ -836,67 +839,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color theme="1"/>
@@ -1018,10 +961,10 @@
   </sortState>
   <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{DF50937B-70CE-4AEE-A127-C34E442E7C61}" name="Jugador" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="14"/>
     <tableColumn id="6" xr3:uid="{1779677D-9229-4A65-A24A-6775E26635BD}" name="Edad 2024"/>
     <tableColumn id="7" xr3:uid="{C7098E7A-A8F5-43C9-A363-2554E8FBB7B3}" name="Pais"/>
     <tableColumn id="8" xr3:uid="{7D8FBA46-C76E-4DB4-B88D-B9B8EDAA5462}" name="Nombres"/>
@@ -1030,16 +973,16 @@
     <tableColumn id="11" xr3:uid="{A731302C-3B92-4B73-9269-9251FFF431F7}" name="Minutos"/>
     <tableColumn id="12" xr3:uid="{3D8BAAFF-953C-4951-9189-62EB68ED7AD5}" name="Goles"/>
     <tableColumn id="13" xr3:uid="{C1DAD42C-FAD1-46CD-9986-BF72BCE1C663}" name="Asistencias"/>
-    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="13" totalsRowDxfId="12"/>
     <tableColumn id="15" xr3:uid="{9D730F2E-328A-4494-A682-1BB9B1DAB250}" name="xG. Por partido"/>
     <tableColumn id="16" xr3:uid="{5B84C753-E393-4F3D-B0A0-98D970CA3FEC}" name="xA. Por partido"/>
     <tableColumn id="17" xr3:uid="{1B52557C-9F62-428C-91E9-9F0E11B4F422}" name="Rojas"/>
     <tableColumn id="18" xr3:uid="{0E14E950-7DF2-4515-B85D-A4F9C752C28B}" name="Amarillas"/>
-    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="11" totalsRowDxfId="10"/>
     <tableColumn id="20" xr3:uid="{B764DC06-CAE4-4962-B815-8920EA707CC3}" name="J1 - Rendimiento"/>
-    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="9" totalsRowDxfId="8"/>
     <tableColumn id="22" xr3:uid="{D908F4EA-DBF5-48D1-A49C-6C9FF3E6D4EB}" name="J2 - Rendimiento"/>
-    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="7" totalsRowDxfId="6"/>
     <tableColumn id="24" xr3:uid="{B0AFBAF2-0C32-422F-B101-93952BDD9341}" name="J3 - Rendimiento"/>
     <tableColumn id="25" xr3:uid="{11744F4F-D50A-4354-937A-E6F9873ADF8B}" name="J4 - Minutos"/>
     <tableColumn id="26" xr3:uid="{241981B8-CCE4-4A57-90A2-836FEAC58BA5}" name="J4 - Rendimiento" totalsRowFunction="count"/>
@@ -1355,7 +1298,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D22" sqref="D22"/>
+      <selection pane="topRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3260,10 +3203,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01D9F4C-E000-464C-8ABC-D44BFB0FC070}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3428,6 +3371,29 @@
       <c r="E8" t="s">
         <v>163</v>
       </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3439,7 +3405,7 @@
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3785,7 +3751,7 @@
   <dimension ref="B2:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Eliminar archivo de datos totales 2024 por falta de datos
</commit_message>
<xml_diff>
--- a/ALIANZA LIMA 2024.xlsx
+++ b/ALIANZA LIMA 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8427246B-F457-4338-819F-19C35D318BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC00086D-77D1-462B-A496-C54495D3A657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Categorias!$A$1:$B$40</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Jugadores!$A$1:$Z$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Jugadores!$A$1:$Z$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="243">
   <si>
     <t>POR</t>
   </si>
@@ -261,18 +261,9 @@
     <t>VLX</t>
   </si>
   <si>
-    <t>VLC</t>
-  </si>
-  <si>
     <t>MCO</t>
   </si>
   <si>
-    <t>DC</t>
-  </si>
-  <si>
-    <t>ATT</t>
-  </si>
-  <si>
     <t>Cecilio</t>
   </si>
   <si>
@@ -697,13 +688,97 @@
   </si>
   <si>
     <t>Jornada 8 - Visita vs Cienciano</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t>Carlos Zambrano</t>
+  </si>
+  <si>
+    <t>Jeriel De Santis</t>
+  </si>
+  <si>
+    <t>VEN</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Jeriel</t>
+  </si>
+  <si>
+    <t>De Santis</t>
+  </si>
+  <si>
+    <t>Zambrano</t>
+  </si>
+  <si>
+    <t>Jornada 9 - Local vs Los Chankas</t>
+  </si>
+  <si>
+    <t>Jornada 1 - Local vs Fluminense</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>Puntos resultantes</t>
+  </si>
+  <si>
+    <t>Jornada 10 - Visita vs Carlos Manucci</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>Jornada 2 - Visita vs Cerro Porteño</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>Copa Libertadores</t>
+  </si>
+  <si>
+    <t>Jornada 11 - Local vs Atlético Grau</t>
+  </si>
+  <si>
+    <t>A11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -732,6 +807,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -759,7 +840,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -802,11 +883,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -821,9 +913,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -833,6 +922,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -954,10 +1050,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D01F760-0D73-4C44-A79F-5468B2DB0477}" name="AlianzaLima" displayName="AlianzaLima" ref="A1:AF28">
-  <autoFilter ref="A1:AF28" xr:uid="{7B836082-5DF0-4CBD-82AC-74ABD84EC464}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z27">
-    <sortCondition descending="1" ref="K1:K27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D01F760-0D73-4C44-A79F-5468B2DB0477}" name="AlianzaLima" displayName="AlianzaLima" ref="A1:AF30">
+  <autoFilter ref="A1:AF30" xr:uid="{7B836082-5DF0-4CBD-82AC-74ABD84EC464}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF30">
+    <sortCondition ref="J1:J30"/>
   </sortState>
   <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{DF50937B-70CE-4AEE-A127-C34E442E7C61}" name="Jugador" totalsRowLabel="Total"/>
@@ -1294,11 +1390,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B836082-5DF0-4CBD-82AC-74ABD84EC464}">
-  <dimension ref="A1:AF28"/>
+  <dimension ref="A1:AF30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B29" sqref="B29"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1326,7 +1422,7 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>68</v>
@@ -1355,23 +1451,23 @@
       <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>45</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="O1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="Q1" t="s">
         <v>15</v>
@@ -1379,87 +1475,89 @@
       <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" t="s">
+        <v>112</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="V1" t="s">
         <v>114</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="X1" t="s">
         <v>116</v>
       </c>
-      <c r="V1" t="s">
-        <v>117</v>
-      </c>
-      <c r="W1" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="Y1" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="Y1" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="Z1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA1" s="9" t="s">
-        <v>127</v>
+        <v>120</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="AB1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>168</v>
+        <v>125</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="AD1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="AE1" s="10" t="s">
-        <v>169</v>
+        <v>126</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>166</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="B2" s="5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="E2" s="3"/>
       <c r="F2">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H2" t="s">
-        <v>37</v>
-      </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="K2">
-        <v>469</v>
+        <v>540</v>
       </c>
       <c r="L2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -1471,7 +1569,7 @@
         <v>90</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U2" s="1">
         <v>90</v>
@@ -1483,43 +1581,45 @@
         <v>90</v>
       </c>
       <c r="AA2">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="AC2">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="B3" s="5">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>215</v>
+      </c>
       <c r="F3">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="I3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J3" t="s">
         <v>25</v>
       </c>
       <c r="K3">
-        <v>540</v>
+        <v>426</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1528,10 +1628,10 @@
         <v>0</v>
       </c>
       <c r="N3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -1540,16 +1640,13 @@
         <v>90</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3" s="1">
         <v>90</v>
       </c>
       <c r="W3" s="1">
-        <v>90</v>
-      </c>
-      <c r="Y3">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="AA3">
         <v>90</v>
@@ -1563,30 +1660,34 @@
         <v>99</v>
       </c>
       <c r="B4" s="5">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="F4">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>150</v>
-      </c>
       <c r="K4">
-        <v>384</v>
+        <v>338</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1595,10 +1696,10 @@
         <v>0</v>
       </c>
       <c r="N4" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Q4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -1607,93 +1708,85 @@
         <v>90</v>
       </c>
       <c r="T4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="U4" s="1">
+        <v>72</v>
+      </c>
+      <c r="W4" s="1">
+        <v>14</v>
+      </c>
+      <c r="Y4">
         <v>90</v>
       </c>
-      <c r="V4">
-        <v>-2</v>
-      </c>
-      <c r="W4" s="1">
-        <v>89</v>
-      </c>
-      <c r="X4">
-        <v>2</v>
-      </c>
       <c r="AA4">
-        <v>90</v>
-      </c>
-      <c r="AC4">
-        <v>25</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="B5" s="5">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5">
+        <v>342</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
         <v>26</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5">
-        <v>499</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>3</v>
-      </c>
-      <c r="N5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5" s="1">
-        <v>89</v>
-      </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
-      <c r="U5" s="1">
-        <v>90</v>
-      </c>
       <c r="W5" s="1">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="Y5">
         <v>90</v>
       </c>
       <c r="AA5">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="AC5">
         <v>90</v>
@@ -1701,109 +1794,95 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B6" s="5">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H6" t="s">
-        <v>76</v>
+        <v>122</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="J6" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="K6">
-        <v>506</v>
+        <v>14</v>
       </c>
       <c r="L6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6" s="1">
-        <v>1</v>
-      </c>
+      <c r="N6" s="1"/>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6" s="1">
-        <v>68</v>
-      </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
-      <c r="U6" s="1">
-        <v>90</v>
-      </c>
-      <c r="V6">
-        <v>1.5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S6" s="2"/>
+      <c r="U6" s="2"/>
       <c r="W6" s="1">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="Y6">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="AA6">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="AC6">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="B7" s="5">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>86</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E7" s="3"/>
       <c r="F7">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H7" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="J7" t="s">
         <v>25</v>
       </c>
       <c r="K7">
-        <v>426</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1812,67 +1891,64 @@
         <v>0</v>
       </c>
       <c r="N7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7" s="1">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="T7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7" s="1">
-        <v>90</v>
-      </c>
-      <c r="W7" s="1">
-        <v>66</v>
-      </c>
-      <c r="AA7">
-        <v>90</v>
-      </c>
-      <c r="AC7">
-        <v>90</v>
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B8" s="5">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="H8" t="s">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="J8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="K8">
-        <v>482</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1884,96 +1960,72 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S8" s="1">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="T8">
         <v>0</v>
       </c>
       <c r="U8" s="1">
-        <v>90</v>
-      </c>
-      <c r="W8" s="1">
-        <v>76</v>
-      </c>
-      <c r="Y8">
-        <v>74</v>
-      </c>
-      <c r="AA8">
-        <v>84</v>
-      </c>
-      <c r="AC8">
-        <v>90</v>
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B9" s="5">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E9" s="3"/>
       <c r="F9">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="I9" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="J9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="K9">
-        <v>323</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
-      <c r="N9" s="1">
-        <v>1</v>
-      </c>
+      <c r="N9" s="1"/>
       <c r="Q9">
         <v>0</v>
       </c>
       <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="S9" s="1">
-        <v>90</v>
-      </c>
-      <c r="T9">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S9" s="2"/>
       <c r="U9" s="1">
-        <v>86</v>
-      </c>
-      <c r="W9" s="1">
-        <v>45</v>
-      </c>
-      <c r="Y9">
-        <v>84</v>
-      </c>
-      <c r="AA9">
-        <v>18</v>
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -1981,117 +2033,76 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>216</v>
       </c>
       <c r="B10" s="5">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="F10">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>219</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
+        <v>222</v>
       </c>
       <c r="J10" t="s">
         <v>25</v>
       </c>
-      <c r="K10">
-        <v>215</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>1</v>
-      </c>
-      <c r="S10" s="1">
-        <v>90</v>
-      </c>
-      <c r="T10">
-        <v>1</v>
-      </c>
-      <c r="U10" s="1">
-        <v>64</v>
-      </c>
-      <c r="W10" s="1">
-        <v>45</v>
-      </c>
-      <c r="Y10">
-        <v>16</v>
-      </c>
-      <c r="AA10">
-        <v>0</v>
-      </c>
-      <c r="AC10">
-        <v>0</v>
-      </c>
+      <c r="N10" s="1"/>
+      <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B11" s="5">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>65</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="F11">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="I11" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="K11">
-        <v>338</v>
+        <v>469</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N11" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -2103,263 +2114,221 @@
         <v>90</v>
       </c>
       <c r="T11">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="U11" s="1">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="W11" s="1">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="Y11">
         <v>90</v>
       </c>
       <c r="AA11">
-        <v>72</v>
+        <v>64</v>
+      </c>
+      <c r="AC11">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B12" s="5">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>71</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E12" s="3"/>
       <c r="F12">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H12" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="I12" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="J12" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K12">
-        <v>418</v>
+        <v>506</v>
       </c>
       <c r="L12">
+        <v>3</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
         <v>1</v>
       </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12" s="1">
-        <v>2</v>
-      </c>
       <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
         <v>1</v>
       </c>
-      <c r="R12">
-        <v>2</v>
-      </c>
       <c r="S12" s="1">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="T12">
-        <v>2</v>
-      </c>
-      <c r="U12" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="U12" s="1">
+        <v>90</v>
+      </c>
+      <c r="V12">
+        <v>1.5</v>
+      </c>
       <c r="W12" s="1">
         <v>90</v>
       </c>
       <c r="Y12">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="AA12">
         <v>90</v>
       </c>
       <c r="AC12">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="B13" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>65</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E13" s="3"/>
       <c r="F13">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H13" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="I13" t="s">
-        <v>151</v>
+        <v>42</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="K13">
-        <v>186</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13" s="1">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N13" s="1"/>
       <c r="Q13">
         <v>0</v>
       </c>
       <c r="R13">
         <v>0</v>
       </c>
-      <c r="S13" s="2">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13" s="1">
-        <v>27</v>
-      </c>
-      <c r="W13" s="1">
-        <v>64</v>
-      </c>
-      <c r="Y13">
-        <v>0</v>
-      </c>
-      <c r="AA13">
-        <v>26</v>
-      </c>
-      <c r="AC13">
-        <v>69</v>
-      </c>
+      <c r="S13" s="2"/>
+      <c r="U13" s="2"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>105</v>
       </c>
       <c r="B14" s="5">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>70</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E14" s="3"/>
       <c r="F14">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H14" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="I14" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="J14" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="K14">
-        <v>158</v>
+        <v>0</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14" s="1">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N14" s="1"/>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14">
-        <v>1</v>
-      </c>
-      <c r="S14" s="1">
-        <v>22</v>
-      </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-      <c r="U14" s="1">
-        <v>63</v>
-      </c>
-      <c r="W14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y14">
-        <v>28</v>
-      </c>
-      <c r="AA14">
-        <v>0</v>
-      </c>
-      <c r="AC14">
-        <v>45</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S14" s="2"/>
+      <c r="U14" s="2"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B15" s="5">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>86</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H15" t="s">
-        <v>53</v>
+        <v>138</v>
       </c>
       <c r="I15" t="s">
-        <v>54</v>
+        <v>139</v>
       </c>
       <c r="J15" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="K15">
-        <v>342</v>
+        <v>19</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -2367,151 +2336,95 @@
       <c r="M15">
         <v>0</v>
       </c>
-      <c r="N15" s="1">
-        <v>0</v>
-      </c>
+      <c r="N15" s="1"/>
       <c r="Q15">
         <v>0</v>
       </c>
       <c r="R15">
-        <v>1</v>
-      </c>
-      <c r="S15" s="1">
-        <v>1</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15" s="1">
-        <v>26</v>
-      </c>
-      <c r="W15" s="1">
-        <v>45</v>
-      </c>
-      <c r="Y15">
-        <v>90</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S15" s="1"/>
+      <c r="Y15" s="6"/>
       <c r="AA15">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="AC15">
-        <v>90</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>217</v>
       </c>
       <c r="B16" s="5">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>74</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
       <c r="F16">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="G16" t="s">
-        <v>80</v>
+        <v>218</v>
       </c>
       <c r="H16" t="s">
-        <v>33</v>
+        <v>220</v>
       </c>
       <c r="I16" t="s">
-        <v>34</v>
+        <v>221</v>
       </c>
       <c r="J16" t="s">
-        <v>30</v>
-      </c>
-      <c r="K16">
-        <v>232</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="N16" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16" s="1">
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16" s="1">
-        <v>11</v>
-      </c>
-      <c r="W16" s="1">
-        <v>45</v>
-      </c>
-      <c r="Y16">
-        <v>62</v>
-      </c>
-      <c r="AA16">
-        <v>84</v>
-      </c>
-      <c r="AC16">
-        <v>30</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="N16" s="1"/>
+      <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B17" s="5">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="E17" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F17">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H17" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="I17" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="J17" t="s">
         <v>30</v>
       </c>
       <c r="K17">
-        <v>106</v>
+        <v>499</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
+        <v>3</v>
+      </c>
+      <c r="N17" s="1">
         <v>1</v>
       </c>
-      <c r="N17" s="1">
-        <v>0</v>
-      </c>
       <c r="Q17">
         <v>0</v>
       </c>
@@ -2519,56 +2432,60 @@
         <v>0</v>
       </c>
       <c r="S17" s="1">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="U17" s="1">
+        <v>90</v>
+      </c>
       <c r="W17" s="1">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="Y17">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="AA17">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="AC17">
-        <v>21</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B18" s="5">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="3"/>
       <c r="F18">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H18" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J18" t="s">
         <v>30</v>
       </c>
       <c r="K18">
-        <v>38</v>
+        <v>215</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -2576,28 +2493,32 @@
       <c r="M18">
         <v>0</v>
       </c>
-      <c r="N18" s="1"/>
+      <c r="N18" s="1">
+        <v>1</v>
+      </c>
       <c r="Q18">
         <v>0</v>
       </c>
       <c r="R18">
         <v>1</v>
       </c>
-      <c r="S18" s="2"/>
+      <c r="S18" s="1">
+        <v>90</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
       <c r="U18" s="1">
-        <v>18</v>
-      </c>
-      <c r="V18">
-        <v>0.5</v>
+        <v>64</v>
       </c>
       <c r="W18" s="1">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="Y18">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="AA18">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AC18">
         <v>0</v>
@@ -2605,150 +2526,186 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="B19" s="5">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="F19">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H19" t="s">
-        <v>125</v>
+        <v>61</v>
       </c>
       <c r="I19" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="J19" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K19">
-        <v>14</v>
+        <v>186</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
       <c r="Q19">
         <v>0</v>
       </c>
       <c r="R19">
         <v>0</v>
       </c>
-      <c r="S19" s="2"/>
-      <c r="U19" s="2"/>
+      <c r="S19" s="2">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19" s="1">
+        <v>27</v>
+      </c>
       <c r="W19" s="1">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="Y19">
         <v>0</v>
       </c>
       <c r="AA19">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AC19">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B20" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20">
         <v>31</v>
       </c>
       <c r="G20" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" t="s">
+        <v>79</v>
+      </c>
+      <c r="I20" t="s">
         <v>80</v>
       </c>
-      <c r="H20" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" t="s">
-        <v>18</v>
-      </c>
       <c r="J20" t="s">
-        <v>150</v>
+        <v>30</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>482</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
-      <c r="N20" s="1"/>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
       <c r="Q20">
         <v>0</v>
       </c>
       <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="AA20" s="2"/>
-      <c r="AC20" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="S20" s="1">
+        <v>68</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20" s="1">
+        <v>90</v>
+      </c>
+      <c r="W20" s="1">
+        <v>76</v>
+      </c>
+      <c r="Y20">
+        <v>74</v>
+      </c>
+      <c r="AA20">
+        <v>84</v>
+      </c>
+      <c r="AC20" s="12">
+        <v>90</v>
+      </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B21" s="5">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="F21">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H21" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="I21" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="J21" t="s">
-        <v>150</v>
+        <v>30</v>
       </c>
       <c r="K21">
-        <v>150</v>
+        <v>323</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21">
         <v>0</v>
@@ -2757,258 +2714,316 @@
         <v>1</v>
       </c>
       <c r="S21" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21" s="1">
-        <v>0</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="W21" s="1">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="Y21">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="AA21">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AC21">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="B22" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="F22">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H22" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="I22" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="J22" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>418</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S22" s="1">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22" s="1">
-        <v>0</v>
-      </c>
-      <c r="V22">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="U22" s="2"/>
+      <c r="W22" s="1">
+        <v>90</v>
       </c>
       <c r="Y22">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="AA22">
+        <v>90</v>
+      </c>
+      <c r="AC22">
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="B23" s="5">
+        <v>15</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23">
+        <v>28</v>
+      </c>
+      <c r="G23" t="s">
+        <v>77</v>
+      </c>
+      <c r="H23" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23">
-        <v>29</v>
-      </c>
-      <c r="G23" t="s">
-        <v>80</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K23">
+        <v>158</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23" s="1">
+        <v>22</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23" s="1">
+        <v>63</v>
+      </c>
+      <c r="W23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y23">
         <v>28</v>
       </c>
-      <c r="I23" t="s">
-        <v>29</v>
-      </c>
-      <c r="J23" t="s">
-        <v>25</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
-      <c r="S23" s="1">
-        <v>0</v>
-      </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
-      <c r="U23" s="1">
-        <v>0</v>
-      </c>
-      <c r="V23">
-        <v>0</v>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B24" s="5">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="3"/>
       <c r="F24">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I24" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="J24" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>232</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0</v>
+      </c>
       <c r="Q24">
         <v>0</v>
       </c>
       <c r="R24">
         <v>0</v>
       </c>
-      <c r="S24" s="2"/>
-      <c r="U24" s="2"/>
+      <c r="S24" s="1">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24" s="1">
+        <v>11</v>
+      </c>
+      <c r="W24" s="1">
+        <v>45</v>
+      </c>
+      <c r="Y24">
+        <v>62</v>
+      </c>
+      <c r="AA24">
+        <v>84</v>
+      </c>
+      <c r="AC24">
+        <v>30</v>
+      </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B25" s="5">
+        <v>7</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25">
         <v>24</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25">
-        <v>17</v>
-      </c>
       <c r="G25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H25" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="I25" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J25" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0</v>
+      </c>
       <c r="Q25">
         <v>0</v>
       </c>
       <c r="R25">
         <v>0</v>
       </c>
-      <c r="S25" s="2"/>
+      <c r="S25" s="1">
+        <v>22</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
       <c r="U25" s="2"/>
+      <c r="W25" s="1">
+        <v>26</v>
+      </c>
+      <c r="Y25">
+        <v>11</v>
+      </c>
+      <c r="AA25">
+        <v>26</v>
+      </c>
+      <c r="AC25">
+        <v>21</v>
+      </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="B26" s="5">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>71</v>
@@ -3018,19 +3033,19 @@
         <v>23</v>
       </c>
       <c r="G26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H26" t="s">
-        <v>138</v>
+        <v>49</v>
       </c>
       <c r="I26" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="J26" t="s">
         <v>30</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -3038,52 +3053,61 @@
       <c r="M26">
         <v>0</v>
       </c>
-      <c r="N26" s="1">
-        <v>0</v>
-      </c>
+      <c r="N26" s="1"/>
       <c r="Q26">
         <v>0</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26" s="2"/>
-      <c r="T26">
-        <v>0</v>
-      </c>
-      <c r="U26" s="2"/>
+      <c r="U26" s="1">
+        <v>18</v>
+      </c>
       <c r="V26">
+        <v>0.5</v>
+      </c>
+      <c r="W26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <v>10</v>
+      </c>
+      <c r="AA26">
+        <v>10</v>
+      </c>
+      <c r="AC26">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="B27" s="5">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H27" t="s">
-        <v>82</v>
+        <v>135</v>
       </c>
       <c r="I27" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="J27" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -3094,7 +3118,9 @@
       <c r="M27">
         <v>0</v>
       </c>
-      <c r="N27" s="1"/>
+      <c r="N27" s="1">
+        <v>0</v>
+      </c>
       <c r="Q27">
         <v>0</v>
       </c>
@@ -3102,72 +3128,204 @@
         <v>0</v>
       </c>
       <c r="S27" s="2"/>
-      <c r="U27" s="1">
-        <v>0</v>
-      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27" s="2"/>
       <c r="V27">
-        <v>0</v>
-      </c>
-      <c r="AC27">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="B28" s="5">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>75</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28">
+        <v>25</v>
+      </c>
+      <c r="G28" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" t="s">
+        <v>147</v>
+      </c>
+      <c r="K28">
+        <v>384</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>2</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28" s="1">
+        <v>90</v>
+      </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
+      <c r="U28" s="1">
+        <v>90</v>
+      </c>
+      <c r="V28">
+        <v>-2</v>
+      </c>
+      <c r="W28" s="1">
+        <v>89</v>
+      </c>
+      <c r="X28">
+        <v>2</v>
+      </c>
+      <c r="AA28">
+        <v>90</v>
+      </c>
+      <c r="AC28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29">
+        <v>31</v>
+      </c>
+      <c r="G29" t="s">
+        <v>77</v>
+      </c>
+      <c r="H29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" t="s">
         <v>18</v>
       </c>
-      <c r="G28" t="s">
-        <v>80</v>
-      </c>
-      <c r="H28" t="s">
-        <v>141</v>
-      </c>
-      <c r="I28" t="s">
-        <v>142</v>
-      </c>
-      <c r="J28" t="s">
-        <v>39</v>
-      </c>
-      <c r="K28">
+      <c r="J29" t="s">
+        <v>147</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1"/>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="AA29" s="2"/>
+      <c r="AC29" s="11"/>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="5">
+        <v>12</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30">
+        <v>22</v>
+      </c>
+      <c r="G30" t="s">
+        <v>77</v>
+      </c>
+      <c r="H30" t="s">
         <v>19</v>
       </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28" s="1"/>
-      <c r="Q28">
-        <v>0</v>
-      </c>
-      <c r="R28">
-        <v>0</v>
-      </c>
-      <c r="S28" s="1"/>
-      <c r="Y28" s="7"/>
-      <c r="AA28">
-        <v>10</v>
-      </c>
-      <c r="AC28">
-        <v>9</v>
+      <c r="I30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30" t="s">
+        <v>147</v>
+      </c>
+      <c r="K30">
+        <v>150</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30" s="1">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30" s="1">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>90</v>
+      </c>
+      <c r="AA30">
+        <v>0</v>
+      </c>
+      <c r="AC30">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="W2:W28 S2:S28 U2:U28 Y2:Y28">
+  <conditionalFormatting sqref="W2:W30 S2:S30 U2:U30 Y2:Y30">
     <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
       <formula>90</formula>
     </cfRule>
@@ -3180,7 +3338,7 @@
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA2:AA28 AC2:AC28">
+  <conditionalFormatting sqref="AA2:AA30 AC2:AC30">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>90</formula>
     </cfRule>
@@ -3203,199 +3361,301 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01D9F4C-E000-464C-8ABC-D44BFB0FC070}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="39.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="11" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>151</v>
+      </c>
+      <c r="B2" t="s">
+        <v>225</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
+        <v>152</v>
+      </c>
+      <c r="B3" t="s">
+        <v>226</v>
       </c>
       <c r="C3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" t="s">
         <v>156</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>159</v>
       </c>
       <c r="D4">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F4">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C5" t="s">
         <v>157</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>160</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
+        <v>155</v>
+      </c>
+      <c r="B6" t="s">
+        <v>229</v>
       </c>
       <c r="C6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>161</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
+        <v>158</v>
+      </c>
+      <c r="B7" t="s">
+        <v>230</v>
       </c>
       <c r="C7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
+        <v>164</v>
+      </c>
+      <c r="B8" t="s">
+        <v>231</v>
       </c>
       <c r="C8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D8">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>217</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
+        <v>214</v>
+      </c>
+      <c r="B9" t="s">
+        <v>232</v>
       </c>
       <c r="C9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F9">
         <v>7</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>223</v>
+      </c>
+      <c r="B10" t="s">
+        <v>233</v>
+      </c>
+      <c r="C10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>224</v>
+      </c>
+      <c r="B11" t="s">
+        <v>234</v>
+      </c>
+      <c r="C11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>240</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>236</v>
+      </c>
+      <c r="B12" t="s">
+        <v>237</v>
+      </c>
+      <c r="C12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>240</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>241</v>
+      </c>
+      <c r="B14" t="s">
+        <v>242</v>
+      </c>
+      <c r="C14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>160</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3404,8 +3664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5DE0E37-A65E-430A-B081-464F0351FE39}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3417,322 +3677,322 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B14" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B15" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B17" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B18" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B19" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B20" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B21" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B22" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B23" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B24" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B25" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B26" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B27" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B28" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B29" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B30" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B31" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B32" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B33" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B34" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B35" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B36" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B37" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>203</v>
+      </c>
+      <c r="B38" t="s">
         <v>206</v>
-      </c>
-      <c r="B38" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B39" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B40" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3766,22 +4026,22 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -3801,37 +4061,37 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Division por posiciones GroneStats
</commit_message>
<xml_diff>
--- a/ALIANZA LIMA 2024.xlsx
+++ b/ALIANZA LIMA 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC00086D-77D1-462B-A496-C54495D3A657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB3E92E-29E5-457E-832F-6EC5C9BBEBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="243">
   <si>
     <t>POR</t>
   </si>
@@ -937,6 +937,46 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color theme="1"/>
       </font>
@@ -996,46 +1036,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1057,10 +1057,10 @@
   </sortState>
   <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{DF50937B-70CE-4AEE-A127-C34E442E7C61}" name="Jugador" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{7C1D37E0-6B69-4854-B666-49C3E8C83692}" name="Dorsal" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{96D9C939-88FB-4445-A3F8-E884EFDC3ED7}" name="Pos_1" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{071A9D16-0DAC-4A32-AA5A-E323DF2C27E6}" name="Pos_2" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{DBACD41F-83FA-4475-9316-7BE5E2AFD077}" name="Pos_3" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{1779677D-9229-4A65-A24A-6775E26635BD}" name="Edad 2024"/>
     <tableColumn id="7" xr3:uid="{C7098E7A-A8F5-43C9-A363-2554E8FBB7B3}" name="Pais"/>
     <tableColumn id="8" xr3:uid="{7D8FBA46-C76E-4DB4-B88D-B9B8EDAA5462}" name="Nombres"/>
@@ -1069,16 +1069,16 @@
     <tableColumn id="11" xr3:uid="{A731302C-3B92-4B73-9269-9251FFF431F7}" name="Minutos"/>
     <tableColumn id="12" xr3:uid="{3D8BAAFF-953C-4951-9189-62EB68ED7AD5}" name="Goles"/>
     <tableColumn id="13" xr3:uid="{C1DAD42C-FAD1-46CD-9986-BF72BCE1C663}" name="Asistencias"/>
-    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{1E46384F-C2ED-4CE6-B038-85028F26317D}" name="Rendimiento temporada" dataDxfId="7" totalsRowDxfId="6"/>
     <tableColumn id="15" xr3:uid="{9D730F2E-328A-4494-A682-1BB9B1DAB250}" name="xG. Por partido"/>
     <tableColumn id="16" xr3:uid="{5B84C753-E393-4F3D-B0A0-98D970CA3FEC}" name="xA. Por partido"/>
     <tableColumn id="17" xr3:uid="{1B52557C-9F62-428C-91E9-9F0E11B4F422}" name="Rojas"/>
     <tableColumn id="18" xr3:uid="{0E14E950-7DF2-4515-B85D-A4F9C752C28B}" name="Amarillas"/>
-    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="19" xr3:uid="{843A31AE-B4ED-4A91-BD23-55D7769CD999}" name="J1 - Minutos" dataDxfId="5" totalsRowDxfId="4"/>
     <tableColumn id="20" xr3:uid="{B764DC06-CAE4-4962-B815-8920EA707CC3}" name="J1 - Rendimiento"/>
-    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="21" xr3:uid="{FB87D0AB-5C50-4970-9F1C-7CC6328C6737}" name="J2 - Minutos" dataDxfId="3" totalsRowDxfId="2"/>
     <tableColumn id="22" xr3:uid="{D908F4EA-DBF5-48D1-A49C-6C9FF3E6D4EB}" name="J2 - Rendimiento"/>
-    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="23" xr3:uid="{33385538-C1E9-49C1-AAC1-969970045173}" name="J3 - Minutos" dataDxfId="1" totalsRowDxfId="0"/>
     <tableColumn id="24" xr3:uid="{B0AFBAF2-0C32-422F-B101-93952BDD9341}" name="J3 - Rendimiento"/>
     <tableColumn id="25" xr3:uid="{11744F4F-D50A-4354-937A-E6F9873ADF8B}" name="J4 - Minutos"/>
     <tableColumn id="26" xr3:uid="{241981B8-CCE4-4A57-90A2-836FEAC58BA5}" name="J4 - Rendimiento" totalsRowFunction="count"/>
@@ -1393,8 +1393,8 @@
   <dimension ref="A1:AF30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L6" sqref="L6"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1531,7 +1531,9 @@
       <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="F2">
         <v>24</v>
       </c>
@@ -1800,12 +1802,14 @@
         <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="3"/>
       <c r="F6">
         <v>21</v>
       </c>
@@ -2075,7 +2079,9 @@
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11">
         <v>40</v>
@@ -2390,7 +2396,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>8</v>
@@ -3326,27 +3332,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W2:W30 S2:S30 U2:U30 Y2:Y30">
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA30 AC2:AC30">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="between">
       <formula>6</formula>
       <formula>89</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="between">
       <formula>0</formula>
       <formula>5</formula>
     </cfRule>

</xml_diff>

<commit_message>
cambios esteticos en radares
</commit_message>
<xml_diff>
--- a/ALIANZA LIMA 2024.xlsx
+++ b/ALIANZA LIMA 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB3E92E-29E5-457E-832F-6EC5C9BBEBC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A9B8A2-29FE-4F34-8F06-DB12B8D17265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
+    <workbookView xWindow="3516" yWindow="2280" windowWidth="17280" windowHeight="8880" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="242">
   <si>
     <t>POR</t>
   </si>
@@ -241,9 +241,6 @@
   </si>
   <si>
     <t>VLI</t>
-  </si>
-  <si>
-    <t>VLD</t>
   </si>
   <si>
     <t>Edad 2024</t>
@@ -1392,9 +1389,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B836082-5DF0-4CBD-82AC-74ABD84EC464}">
   <dimension ref="A1:AF30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C27" sqref="C27"/>
+      <selection pane="topRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1422,10 +1419,10 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1437,7 +1434,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
@@ -1461,13 +1458,13 @@
         <v>45</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" t="s">
         <v>87</v>
-      </c>
-      <c r="O1" t="s">
-        <v>86</v>
-      </c>
-      <c r="P1" t="s">
-        <v>88</v>
       </c>
       <c r="Q1" t="s">
         <v>15</v>
@@ -1476,51 +1473,51 @@
         <v>16</v>
       </c>
       <c r="S1" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T1" t="s">
         <v>111</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" t="s">
         <v>113</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" t="s">
         <v>115</v>
       </c>
-      <c r="X1" t="s">
-        <v>116</v>
-      </c>
       <c r="Y1" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z1" t="s">
         <v>119</v>
       </c>
-      <c r="Z1" t="s">
-        <v>120</v>
-      </c>
       <c r="AA1" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB1" t="s">
         <v>124</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="AD1" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AE1" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="AD1" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE1" s="9" t="s">
-        <v>166</v>
-      </c>
       <c r="AF1" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" s="5">
         <v>2</v>
@@ -1538,7 +1535,7 @@
         <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H2" t="s">
         <v>40</v>
@@ -1591,7 +1588,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" s="5">
         <v>29</v>
@@ -1603,16 +1600,16 @@
         <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F3">
         <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I3" t="s">
         <v>59</v>
@@ -1659,7 +1656,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="5">
         <v>13</v>
@@ -1677,7 +1674,7 @@
         <v>28</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -1727,7 +1724,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" s="5">
         <v>6</v>
@@ -1736,14 +1733,14 @@
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5">
         <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" t="s">
         <v>53</v>
@@ -1796,13 +1793,13 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" s="5">
         <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
@@ -1814,13 +1811,13 @@
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I6" t="s">
         <v>122</v>
-      </c>
-      <c r="I6" t="s">
-        <v>123</v>
       </c>
       <c r="J6" t="s">
         <v>25</v>
@@ -1858,7 +1855,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" s="5">
         <v>4</v>
@@ -1874,7 +1871,7 @@
         <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H7" t="s">
         <v>23</v>
@@ -1921,7 +1918,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" s="5">
         <v>31</v>
@@ -1937,7 +1934,7 @@
         <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H8" t="s">
         <v>28</v>
@@ -1981,7 +1978,7 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" s="5">
         <v>21</v>
@@ -1997,13 +1994,13 @@
         <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J9" t="s">
         <v>25</v>
@@ -2037,7 +2034,7 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B10" s="5">
         <v>55</v>
@@ -2046,7 +2043,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>6</v>
@@ -2055,13 +2052,13 @@
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J10" t="s">
         <v>25</v>
@@ -2071,7 +2068,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B11" s="5">
         <v>9</v>
@@ -2080,14 +2077,14 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11">
         <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H11" t="s">
         <v>37</v>
@@ -2140,7 +2137,7 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B12" s="5">
         <v>30</v>
@@ -2156,13 +2153,13 @@
         <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" t="s">
         <v>73</v>
-      </c>
-      <c r="I12" t="s">
-        <v>74</v>
       </c>
       <c r="J12" t="s">
         <v>39</v>
@@ -2212,7 +2209,7 @@
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" s="5">
         <v>19</v>
@@ -2228,7 +2225,7 @@
         <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H13" t="s">
         <v>35</v>
@@ -2260,7 +2257,7 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14" s="5">
         <v>24</v>
@@ -2276,7 +2273,7 @@
         <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H14" t="s">
         <v>43</v>
@@ -2308,7 +2305,7 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B15" s="5">
         <v>22</v>
@@ -2322,13 +2319,13 @@
         <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H15" t="s">
+        <v>137</v>
+      </c>
+      <c r="I15" t="s">
         <v>138</v>
-      </c>
-      <c r="I15" t="s">
-        <v>139</v>
       </c>
       <c r="J15" t="s">
         <v>39</v>
@@ -2360,7 +2357,7 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B16" s="5">
         <v>18</v>
@@ -2374,13 +2371,13 @@
         <v>21</v>
       </c>
       <c r="G16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H16" t="s">
+        <v>219</v>
+      </c>
+      <c r="I16" t="s">
         <v>220</v>
-      </c>
-      <c r="I16" t="s">
-        <v>221</v>
       </c>
       <c r="J16" t="s">
         <v>39</v>
@@ -2390,7 +2387,7 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B17" s="5">
         <v>26</v>
@@ -2408,7 +2405,7 @@
         <v>26</v>
       </c>
       <c r="G17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H17" t="s">
         <v>46</v>
@@ -2461,25 +2458,25 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B18" s="5">
         <v>20</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18">
         <v>26</v>
       </c>
       <c r="G18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H18" t="s">
         <v>41</v>
@@ -2532,7 +2529,7 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19" s="5">
         <v>11</v>
@@ -2550,13 +2547,13 @@
         <v>24</v>
       </c>
       <c r="G19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H19" t="s">
         <v>61</v>
       </c>
       <c r="I19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J19" t="s">
         <v>30</v>
@@ -2603,29 +2600,29 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="5">
         <v>10</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20">
         <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H20" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" t="s">
         <v>79</v>
-      </c>
-      <c r="I20" t="s">
-        <v>80</v>
       </c>
       <c r="J20" t="s">
         <v>30</v>
@@ -2672,25 +2669,25 @@
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" s="5">
         <v>27</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="F21">
         <v>19</v>
       </c>
       <c r="G21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H21" t="s">
         <v>55</v>
@@ -2743,25 +2740,25 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="5">
         <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="F22">
         <v>31</v>
       </c>
       <c r="G22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H22" t="s">
         <v>57</v>
@@ -2812,25 +2809,25 @@
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B23" s="5">
         <v>15</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="F23">
         <v>28</v>
       </c>
       <c r="G23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H23" t="s">
         <v>31</v>
@@ -2883,16 +2880,16 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" s="5">
         <v>8</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>9</v>
@@ -2901,7 +2898,7 @@
         <v>34</v>
       </c>
       <c r="G24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H24" t="s">
         <v>33</v>
@@ -2954,7 +2951,7 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B25" s="5">
         <v>7</v>
@@ -2972,7 +2969,7 @@
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H25" t="s">
         <v>21</v>
@@ -3023,23 +3020,23 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" s="5">
         <v>14</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26">
         <v>23</v>
       </c>
       <c r="G26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H26" t="s">
         <v>49</v>
@@ -3088,29 +3085,29 @@
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B27" s="5">
         <v>16</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27">
         <v>23</v>
       </c>
       <c r="G27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H27" t="s">
+        <v>134</v>
+      </c>
+      <c r="I27" t="s">
         <v>135</v>
-      </c>
-      <c r="I27" t="s">
-        <v>136</v>
       </c>
       <c r="J27" t="s">
         <v>30</v>
@@ -3144,7 +3141,7 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B28" s="5">
         <v>32</v>
@@ -3158,7 +3155,7 @@
         <v>25</v>
       </c>
       <c r="G28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H28" t="s">
         <v>21</v>
@@ -3167,7 +3164,7 @@
         <v>22</v>
       </c>
       <c r="J28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K28">
         <v>384</v>
@@ -3214,7 +3211,7 @@
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B29" s="5">
         <v>1</v>
@@ -3228,7 +3225,7 @@
         <v>31</v>
       </c>
       <c r="G29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H29" t="s">
         <v>17</v>
@@ -3237,7 +3234,7 @@
         <v>18</v>
       </c>
       <c r="J29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -3262,7 +3259,7 @@
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B30" s="5">
         <v>12</v>
@@ -3276,7 +3273,7 @@
         <v>22</v>
       </c>
       <c r="G30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H30" t="s">
         <v>19</v>
@@ -3285,7 +3282,7 @@
         <v>20</v>
       </c>
       <c r="J30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K30">
         <v>150</v>
@@ -3382,42 +3379,42 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>163</v>
-      </c>
       <c r="G1" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F2">
         <v>4</v>
@@ -3425,19 +3422,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -3445,19 +3442,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F4">
         <v>7</v>
@@ -3465,19 +3462,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -3485,19 +3482,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" t="s">
         <v>155</v>
-      </c>
-      <c r="B6" t="s">
-        <v>229</v>
-      </c>
-      <c r="C6" t="s">
-        <v>156</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -3505,19 +3502,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -3525,19 +3522,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D8">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F8">
         <v>5</v>
@@ -3545,19 +3542,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F9">
         <v>7</v>
@@ -3565,36 +3562,36 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D10">
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -3605,36 +3602,36 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" t="s">
         <v>236</v>
       </c>
-      <c r="B12" t="s">
-        <v>237</v>
-      </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D12">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>237</v>
+      </c>
+      <c r="B13" t="s">
         <v>238</v>
       </c>
-      <c r="B13" t="s">
-        <v>239</v>
-      </c>
       <c r="C13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13">
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -3645,19 +3642,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B14" t="s">
         <v>241</v>
       </c>
-      <c r="B14" t="s">
-        <v>242</v>
-      </c>
       <c r="C14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D14">
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3683,322 +3680,322 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B28" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B34" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B37" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B38" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>204</v>
+      </c>
+      <c r="B40" t="s">
         <v>205</v>
-      </c>
-      <c r="B40" t="s">
-        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -4032,22 +4029,22 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
         <v>91</v>
       </c>
-      <c r="C2" t="s">
-        <v>92</v>
-      </c>
       <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
         <v>84</v>
       </c>
-      <c r="E2" t="s">
-        <v>85</v>
-      </c>
       <c r="F2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" t="s">
         <v>89</v>
-      </c>
-      <c r="G2" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -4067,37 +4064,37 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modificaciones locales para obtener mas datos de liga
</commit_message>
<xml_diff>
--- a/ALIANZA LIMA 2024.xlsx
+++ b/ALIANZA LIMA 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47552F66-8C7B-45B4-8F16-93A8E9349128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AACF836-EC59-4C3A-BB04-EB7603B96E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{26825E93-4751-42C3-94B0-F06FF449CFAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Jugadores" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="255">
   <si>
     <t>POR</t>
   </si>
@@ -2070,7 +2070,12 @@
       <c:pivotFmt>
         <c:idx val="36"/>
         <c:spPr>
-          <a:ln w="31750" cap="rnd">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="31750" cap="rnd" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
@@ -2124,7 +2129,12 @@
       <c:pivotFmt>
         <c:idx val="37"/>
         <c:spPr>
-          <a:ln w="31750" cap="rnd">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="31750" cap="rnd" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
@@ -2186,7 +2196,12 @@
       <c:pivotFmt>
         <c:idx val="38"/>
         <c:spPr>
-          <a:ln w="31750" cap="rnd">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="31750" cap="rnd" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
@@ -2250,7 +2265,12 @@
       <c:pivotFmt>
         <c:idx val="39"/>
         <c:spPr>
-          <a:ln w="31750" cap="rnd">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="31750" cap="rnd" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
@@ -2333,7 +2353,12 @@
               <a:schemeClr val="accent3"/>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -2342,7 +2367,12 @@
       <c:pivotFmt>
         <c:idx val="41"/>
         <c:spPr>
-          <a:ln w="31750" cap="rnd">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="31750" cap="rnd" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
@@ -2404,7 +2434,12 @@
       <c:pivotFmt>
         <c:idx val="42"/>
         <c:spPr>
-          <a:ln w="31750" cap="rnd">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="31750" cap="rnd" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
@@ -2466,7 +2501,12 @@
       <c:pivotFmt>
         <c:idx val="43"/>
         <c:spPr>
-          <a:ln w="31750" cap="rnd">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="31750" cap="rnd" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
             </a:solidFill>
@@ -2478,7 +2518,12 @@
       <c:pivotFmt>
         <c:idx val="44"/>
         <c:spPr>
-          <a:ln w="31750" cap="rnd">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="31750" cap="rnd" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx2"/>
             </a:solidFill>
@@ -4847,7 +4892,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31DE15C8-33D5-41EF-B755-EF5BFE0EFEE8}" name="TablaDinámica1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31DE15C8-33D5-41EF-B755-EF5BFE0EFEE8}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A5:D40" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="17">
     <pivotField axis="axisRow" showAll="0">
@@ -7544,10 +7589,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01D9F4C-E000-464C-8ABC-D44BFB0FC070}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="N18" sqref="N18"/>
+      <selection pane="topRight" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8800,16 +8845,39 @@
       <c r="E24" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="5"/>
+      <c r="F24" s="31">
+        <v>3</v>
+      </c>
+      <c r="G24" s="15">
+        <v>2</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="I24" s="3">
         <v>5</v>
       </c>
       <c r="J24" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="K24" s="3"/>
+      <c r="K24" s="3">
+        <v>4</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+      <c r="M24">
+        <v>14</v>
+      </c>
+      <c r="N24">
+        <v>6</v>
+      </c>
+      <c r="O24">
+        <v>10</v>
+      </c>
+      <c r="P24">
+        <v>2</v>
+      </c>
       <c r="Q24">
         <v>18</v>
       </c>
@@ -8901,7 +8969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC1C93F-25B9-4A4F-81F3-86CA4803A87E}">
   <dimension ref="A3:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>

</xml_diff>